<commit_message>
Added table for I/O testing
git-svn-id: file://localhost/tmp/svn2git/svn@3680 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/data-intensive-bio/Results.xlsx
+++ b/papers/data-intensive-bio/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="27980" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="27960" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="24">
   <si>
     <t>Type</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Size of Read files(GB)</t>
   </si>
   <si>
-    <t>Size of Read files(MB)</t>
-  </si>
-  <si>
     <t>Varying the Number of threads</t>
   </si>
   <si>
@@ -79,6 +76,21 @@
   </si>
   <si>
     <t>Varying the Number of Read Files with different number of Index files</t>
+  </si>
+  <si>
+    <t>Understanding I/O</t>
+  </si>
+  <si>
+    <t>painter</t>
+  </si>
+  <si>
+    <t>Number of cores/bfast-match</t>
+  </si>
+  <si>
+    <t>Number of bfast matches for this test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of nodes </t>
   </si>
 </sst>
 </file>
@@ -161,7 +173,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -173,6 +185,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -211,7 +233,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="10"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -228,6 +250,11 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="10" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
@@ -246,6 +273,11 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -658,10 +690,10 @@
       <xdr:rowOff>209550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -683,15 +715,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:colOff>406400</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>222250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1035,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1048,12 +1080,13 @@
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27" customHeight="1" thickBot="1">
       <c r="A1" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="59" customHeight="1" thickTop="1" thickBot="1">
@@ -1073,7 +1106,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
@@ -1194,7 +1227,7 @@
     </row>
     <row r="9" spans="1:9" ht="20" thickBot="1">
       <c r="A9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="50" thickTop="1" thickBot="1">
@@ -1243,7 +1276,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="H11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I11">
         <v>4</v>
@@ -1266,7 +1299,7 @@
         <v>1.2</v>
       </c>
       <c r="H12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I12">
         <v>4</v>
@@ -1289,18 +1322,18 @@
         <v>0.73199999999999998</v>
       </c>
       <c r="H13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I13">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="20" thickBot="1">
+    <row r="17" spans="1:12" ht="20" thickBot="1">
       <c r="A17" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="50" thickTop="1" thickBot="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="50" thickTop="1" thickBot="1">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -1314,7 +1347,7 @@
         <v>3</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>12</v>
@@ -1329,7 +1362,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="16" thickTop="1">
+    <row r="19" spans="1:12" ht="16" thickTop="1">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1343,7 +1376,7 @@
         <v>37</v>
       </c>
       <c r="E19">
-        <v>229</v>
+        <v>0.22900000000000001</v>
       </c>
       <c r="F19">
         <v>3539</v>
@@ -1355,7 +1388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1369,7 +1402,7 @@
         <v>37</v>
       </c>
       <c r="E20">
-        <v>229</v>
+        <v>0.22900000000000001</v>
       </c>
       <c r="F20">
         <v>2908</v>
@@ -1381,7 +1414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1395,7 +1428,7 @@
         <v>37</v>
       </c>
       <c r="E21">
-        <v>229</v>
+        <v>0.22900000000000001</v>
       </c>
       <c r="F21">
         <v>2834</v>
@@ -1407,7 +1440,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1421,7 +1454,7 @@
         <v>37</v>
       </c>
       <c r="E22">
-        <v>229</v>
+        <v>0.22900000000000001</v>
       </c>
       <c r="F22">
         <v>2718</v>
@@ -1433,7 +1466,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1447,7 +1480,7 @@
         <v>37</v>
       </c>
       <c r="E23">
-        <v>229</v>
+        <v>0.22900000000000001</v>
       </c>
       <c r="F23">
         <v>2716</v>
@@ -1459,7 +1492,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1473,7 +1506,7 @@
         <v>37</v>
       </c>
       <c r="E24">
-        <v>229</v>
+        <v>0.22900000000000001</v>
       </c>
       <c r="F24">
         <v>2725</v>
@@ -1485,7 +1518,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1499,7 +1532,7 @@
         <v>37</v>
       </c>
       <c r="E25">
-        <v>229</v>
+        <v>0.22900000000000001</v>
       </c>
       <c r="F25">
         <v>2715</v>
@@ -1511,7 +1544,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="49" thickBot="1">
+    <row r="28" spans="1:12" ht="20" thickBot="1">
+      <c r="A28" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="66" thickTop="1" thickBot="1">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -1525,7 +1563,7 @@
         <v>3</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>12</v>
@@ -1539,8 +1577,17 @@
       <c r="I29" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="16" thickTop="1">
+      <c r="J29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="16" thickTop="1">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -1551,22 +1598,28 @@
         <v>4</v>
       </c>
       <c r="D30">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="E30">
-        <v>229</v>
-      </c>
-      <c r="F30">
-        <v>2908</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H30" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I30">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>4</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1577,22 +1630,92 @@
         <v>4</v>
       </c>
       <c r="D31">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="E31">
-        <v>229</v>
-      </c>
-      <c r="F31">
-        <v>2834</v>
+        <v>1.2</v>
       </c>
       <c r="H31" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I31">
+        <v>2</v>
+      </c>
+      <c r="J31">
+        <v>2</v>
+      </c>
+      <c r="K31">
+        <v>2</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="5:5">
+      <c r="E32">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="H32" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>4</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>40</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>8</v>
+      </c>
+      <c r="E33">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="H33" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>4</v>
+      </c>
+      <c r="K33">
+        <v>2</v>
+      </c>
+      <c r="L33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="E36" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding cloud test run
git-svn-id: file://localhost/tmp/svn2git/svn@3724 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/data-intensive-bio/Results.xlsx
+++ b/papers/data-intensive-bio/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="129"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16640" tabRatio="129"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="63">
   <si>
     <t>Type</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Number of Read files</t>
   </si>
   <si>
-    <t>1.9GB</t>
-  </si>
-  <si>
     <t>Time to Process all Read  files</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
     <t xml:space="preserve"> Size of each Read files(GB)</t>
   </si>
   <si>
-    <t>Size of all Index files</t>
-  </si>
-  <si>
     <t>QB</t>
   </si>
   <si>
@@ -205,13 +199,22 @@
   </si>
   <si>
     <t xml:space="preserve">Painter  4 core, RAM 4 GB </t>
+  </si>
+  <si>
+    <t>3.3GB</t>
+  </si>
+  <si>
+    <t>B.glumae</t>
+  </si>
+  <si>
+    <t>Size of all Index files(GB)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -278,25 +281,13 @@
       <color rgb="FF292929"/>
       <name val="Courier"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -335,7 +326,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="135">
+  <cellStyleXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -448,7 +439,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -472,7 +490,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -492,15 +510,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="79"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="112" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="112"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="112" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="135">
+  <cellStyles count="162">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -555,17 +566,31 @@
     <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="10" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
@@ -622,18 +647,31 @@
     <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Neutral" xfId="112" builtinId="28"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Warning Text" xfId="79" builtinId="11"/>
   </cellStyles>
@@ -686,8 +724,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.200877958785014"/>
-          <c:y val="0.15370390068622"/>
+          <c:x val="0.205472139489455"/>
+          <c:y val="0.145777884105306"/>
           <c:w val="0.665655404706682"/>
           <c:h val="0.680482408053424"/>
         </c:manualLayout>
@@ -787,7 +825,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$11:$E$14</c:f>
+              <c:f>Sheet1!$E$16:$E$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -808,7 +846,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$11:$F$14</c:f>
+              <c:f>Sheet1!$F$16:$F$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -837,11 +875,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="481437992"/>
-        <c:axId val="481446440"/>
+        <c:axId val="517892040"/>
+        <c:axId val="511854824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="481437992"/>
+        <c:axId val="517892040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,12 +908,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="481446440"/>
+        <c:crossAx val="511854824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="481446440"/>
+        <c:axId val="511854824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -909,7 +947,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="481437992"/>
+        <c:crossAx val="517892040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -995,7 +1033,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$17</c:f>
+              <c:f>Sheet1!$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1020,7 +1058,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$I$19:$I$25</c:f>
+              <c:f>Sheet1!$I$24:$I$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1050,7 +1088,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$19:$F$25</c:f>
+              <c:f>Sheet1!$F$24:$F$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1088,11 +1126,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="101563896"/>
-        <c:axId val="101571016"/>
+        <c:axId val="511899928"/>
+        <c:axId val="517702760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101563896"/>
+        <c:axId val="511899928"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -1122,12 +1160,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101571016"/>
+        <c:crossAx val="517702760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101571016"/>
+        <c:axId val="517702760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1156,7 +1194,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101563896"/>
+        <c:crossAx val="511899928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1252,7 +1290,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$K$30:$K$32</c:f>
+              <c:f>Sheet1!$K$39:$K$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1270,7 +1308,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$30:$F$32</c:f>
+              <c:f>Sheet1!$F$39:$F$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1296,11 +1334,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="101596744"/>
-        <c:axId val="101601304"/>
+        <c:axId val="517905832"/>
+        <c:axId val="511807544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101596744"/>
+        <c:axId val="517905832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1310,13 +1348,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101601304"/>
+        <c:crossAx val="511807544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101601304"/>
+        <c:axId val="511807544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1326,7 +1364,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101596744"/>
+        <c:crossAx val="517905832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1353,10 +1391,10 @@
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1378,15 +1416,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>825500</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1415,7 +1453,7 @@
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>698500</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1760,10 +1798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O95"/>
+  <dimension ref="A1:O104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1787,19 +1825,19 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" thickBot="1">
       <c r="A1" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="59" customHeight="1" thickTop="1" thickBot="1">
@@ -1810,45 +1848,45 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="16" thickTop="1">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>40</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
+      <c r="C3">
+        <v>1.9</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -1861,7 +1899,7 @@
         <v>36942</v>
       </c>
       <c r="H3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I3">
         <v>4</v>
@@ -1879,13 +1917,13 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>40</v>
       </c>
-      <c r="C4" t="s">
-        <v>3</v>
+      <c r="C4">
+        <v>1.9</v>
       </c>
       <c r="D4">
         <v>8</v>
@@ -1897,7 +1935,7 @@
         <v>18603</v>
       </c>
       <c r="H4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I4">
         <v>4</v>
@@ -1915,13 +1953,13 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>40</v>
       </c>
-      <c r="C5" t="s">
-        <v>3</v>
+      <c r="C5">
+        <v>1.9</v>
       </c>
       <c r="D5">
         <v>12</v>
@@ -1934,7 +1972,7 @@
         <v>11916</v>
       </c>
       <c r="H5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I5">
         <v>4</v>
@@ -1952,13 +1990,13 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>40</v>
       </c>
-      <c r="C6" t="s">
-        <v>3</v>
+      <c r="C6">
+        <v>1.9</v>
       </c>
       <c r="D6">
         <v>37</v>
@@ -1971,7 +2009,7 @@
         <v>3841</v>
       </c>
       <c r="H6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I6">
         <v>4</v>
@@ -1987,412 +2025,263 @@
         <v>142117</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="20" thickBot="1">
-      <c r="A9" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="50" thickTop="1" thickBot="1">
-      <c r="A10" s="1" t="s">
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7">
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <v>0.439</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="20" thickBot="1">
+      <c r="A14" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="50" thickTop="1" thickBot="1">
+      <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="C15" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="E15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="16" thickTop="1">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>1.9</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F16">
+        <v>8810</v>
+      </c>
+      <c r="H16" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16" s="7">
+        <v>4</v>
+      </c>
+      <c r="K16" s="8">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <f>D16*F16</f>
+        <v>35240</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>1.9</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>1.2</v>
+      </c>
+      <c r="F17">
+        <v>4428</v>
+      </c>
+      <c r="H17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17" s="7">
+        <v>4</v>
+      </c>
+      <c r="K17" s="7">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <f>D17*F17</f>
+        <v>35424</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>1.9</v>
+      </c>
+      <c r="D18">
+        <v>12</v>
+      </c>
+      <c r="E18">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="F18">
+        <v>2855</v>
+      </c>
+      <c r="H18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="J18" s="7">
+        <v>4</v>
+      </c>
+      <c r="K18" s="7">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <f>D18*F18</f>
+        <v>34260</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="7">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>1.9</v>
+      </c>
+      <c r="D19" s="7">
+        <v>37</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="F19" s="7">
+        <v>936</v>
+      </c>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I19" s="7">
+        <v>4</v>
+      </c>
+      <c r="J19" s="7">
+        <v>4</v>
+      </c>
+      <c r="K19" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+    </row>
+    <row r="22" spans="1:12" ht="20" thickBot="1">
+      <c r="A22" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="66" thickTop="1" thickBot="1">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="16" thickTop="1">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="G23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F11">
-        <v>8810</v>
-      </c>
-      <c r="H11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11">
-        <v>4</v>
-      </c>
-      <c r="J11" s="7">
-        <v>4</v>
-      </c>
-      <c r="K11" s="8">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <f>D11*F11</f>
-        <v>35240</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12">
+      <c r="H23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E12">
-        <v>1.2</v>
-      </c>
-      <c r="F12">
-        <v>4428</v>
-      </c>
-      <c r="H12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12">
-        <v>4</v>
-      </c>
-      <c r="J12" s="7">
-        <v>4</v>
-      </c>
-      <c r="K12" s="7">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <f>D12*F12</f>
-        <v>35424</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13">
-        <v>12</v>
-      </c>
-      <c r="E13">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="F13">
-        <v>2855</v>
-      </c>
-      <c r="H13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13">
-        <v>4</v>
-      </c>
-      <c r="J13" s="7">
-        <v>4</v>
-      </c>
-      <c r="K13" s="7">
-        <v>1</v>
-      </c>
-      <c r="L13">
-        <f>D13*F13</f>
-        <v>34260</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="7">
-        <v>10</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="7">
-        <v>37</v>
-      </c>
-      <c r="E14" s="7">
-        <v>0.22900000000000001</v>
-      </c>
-      <c r="F14" s="7">
-        <v>936</v>
-      </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7" t="s">
+      <c r="J23" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="16" thickTop="1">
+      <c r="A24" t="s">
         <v>6</v>
-      </c>
-      <c r="I14" s="7">
-        <v>4</v>
-      </c>
-      <c r="J14" s="7">
-        <v>4</v>
-      </c>
-      <c r="K14" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-    </row>
-    <row r="17" spans="1:13" ht="20" thickBot="1">
-      <c r="A17" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="66" thickTop="1" thickBot="1">
-      <c r="A18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="16" thickTop="1">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19">
-        <v>40</v>
-      </c>
-      <c r="C19" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19">
-        <v>37</v>
-      </c>
-      <c r="E19">
-        <v>0.22900000000000001</v>
-      </c>
-      <c r="F19">
-        <v>3539</v>
-      </c>
-      <c r="H19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I19">
-        <v>1</v>
-      </c>
-      <c r="J19" s="7">
-        <v>12</v>
-      </c>
-      <c r="K19" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20">
-        <v>40</v>
-      </c>
-      <c r="C20" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20">
-        <v>37</v>
-      </c>
-      <c r="E20">
-        <v>0.22900000000000001</v>
-      </c>
-      <c r="F20">
-        <v>2908</v>
-      </c>
-      <c r="H20" t="s">
-        <v>8</v>
-      </c>
-      <c r="I20">
-        <v>4</v>
-      </c>
-      <c r="J20" s="7">
-        <v>12</v>
-      </c>
-      <c r="K20" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21">
-        <v>40</v>
-      </c>
-      <c r="C21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21">
-        <v>37</v>
-      </c>
-      <c r="E21">
-        <v>0.22900000000000001</v>
-      </c>
-      <c r="F21">
-        <v>2834</v>
-      </c>
-      <c r="H21" t="s">
-        <v>8</v>
-      </c>
-      <c r="I21">
-        <v>8</v>
-      </c>
-      <c r="J21" s="7">
-        <v>12</v>
-      </c>
-      <c r="K21" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22">
-        <v>40</v>
-      </c>
-      <c r="C22" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22">
-        <v>37</v>
-      </c>
-      <c r="E22">
-        <v>0.22900000000000001</v>
-      </c>
-      <c r="F22">
-        <v>2718</v>
-      </c>
-      <c r="H22" t="s">
-        <v>8</v>
-      </c>
-      <c r="I22">
-        <v>12</v>
-      </c>
-      <c r="J22" s="7">
-        <v>12</v>
-      </c>
-      <c r="K22" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23">
-        <v>40</v>
-      </c>
-      <c r="C23" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23">
-        <v>37</v>
-      </c>
-      <c r="E23">
-        <v>0.22900000000000001</v>
-      </c>
-      <c r="F23">
-        <v>2716</v>
-      </c>
-      <c r="H23" t="s">
-        <v>8</v>
-      </c>
-      <c r="I23">
-        <v>16</v>
-      </c>
-      <c r="J23" s="7">
-        <v>12</v>
-      </c>
-      <c r="K23" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" t="s">
-        <v>7</v>
       </c>
       <c r="B24">
         <v>40</v>
       </c>
-      <c r="C24" t="s">
-        <v>3</v>
+      <c r="C24">
+        <v>1.9</v>
       </c>
       <c r="D24">
         <v>37</v>
@@ -2401,30 +2290,30 @@
         <v>0.22900000000000001</v>
       </c>
       <c r="F24">
-        <v>2725</v>
+        <v>3539</v>
       </c>
       <c r="H24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I24">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="J24" s="7">
         <v>12</v>
       </c>
-      <c r="K24" s="7">
+      <c r="K24" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25">
         <v>40</v>
       </c>
-      <c r="C25" t="s">
-        <v>3</v>
+      <c r="C25">
+        <v>1.9</v>
       </c>
       <c r="D25">
         <v>37</v>
@@ -2433,13 +2322,13 @@
         <v>0.22900000000000001</v>
       </c>
       <c r="F25">
-        <v>2715</v>
+        <v>2908</v>
       </c>
       <c r="H25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I25">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="J25" s="7">
         <v>12</v>
@@ -2448,711 +2337,761 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="20" thickBot="1">
-      <c r="A28" s="4" t="s">
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <v>40</v>
+      </c>
+      <c r="C26">
+        <v>1.9</v>
+      </c>
+      <c r="D26">
+        <v>37</v>
+      </c>
+      <c r="E26">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="F26">
+        <v>2834</v>
+      </c>
+      <c r="H26" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26">
+        <v>8</v>
+      </c>
+      <c r="J26" s="7">
+        <v>12</v>
+      </c>
+      <c r="K26" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>40</v>
+      </c>
+      <c r="C27">
+        <v>1.9</v>
+      </c>
+      <c r="D27">
+        <v>37</v>
+      </c>
+      <c r="E27">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="F27">
+        <v>2718</v>
+      </c>
+      <c r="H27" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27">
+        <v>12</v>
+      </c>
+      <c r="J27" s="7">
+        <v>12</v>
+      </c>
+      <c r="K27" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>40</v>
+      </c>
+      <c r="C28">
+        <v>1.9</v>
+      </c>
+      <c r="D28">
+        <v>37</v>
+      </c>
+      <c r="E28">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="F28">
+        <v>2716</v>
+      </c>
+      <c r="H28" t="s">
+        <v>7</v>
+      </c>
+      <c r="I28">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" ht="50" thickTop="1" thickBot="1">
-      <c r="A29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="J28" s="7">
+        <v>12</v>
+      </c>
+      <c r="K28" s="7">
         <v>1</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M29" s="1"/>
-    </row>
-    <row r="30" spans="1:13" ht="16" thickTop="1">
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>40</v>
+      </c>
+      <c r="C29">
+        <v>1.9</v>
+      </c>
+      <c r="D29">
+        <v>37</v>
+      </c>
+      <c r="E29">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="F29">
+        <v>2725</v>
+      </c>
+      <c r="H29" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29">
+        <v>20</v>
+      </c>
+      <c r="J29" s="7">
+        <v>12</v>
+      </c>
+      <c r="K29" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30">
         <v>40</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30">
+        <v>1.9</v>
+      </c>
+      <c r="D30">
+        <v>37</v>
+      </c>
+      <c r="E30">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="F30">
+        <v>2715</v>
+      </c>
+      <c r="H30" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30">
+        <v>32</v>
+      </c>
+      <c r="J30" s="7">
+        <v>12</v>
+      </c>
+      <c r="K30" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>10</v>
+      </c>
+      <c r="C31">
+        <v>1.9</v>
+      </c>
+      <c r="D31">
+        <v>37</v>
+      </c>
+      <c r="E31">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="F31">
+        <v>662</v>
+      </c>
+      <c r="H31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31">
+        <v>20</v>
+      </c>
+      <c r="J31" s="7">
+        <v>12</v>
+      </c>
+      <c r="K31" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32">
+        <v>37</v>
+      </c>
+      <c r="E32">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="F32">
+        <v>676</v>
+      </c>
+      <c r="H32" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32">
+        <v>32</v>
+      </c>
+      <c r="J32" s="7">
+        <v>12</v>
+      </c>
+      <c r="K32" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="20" thickBot="1">
+      <c r="A37" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="50" thickTop="1" thickBot="1">
+      <c r="A38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D30">
-        <v>4</v>
-      </c>
-      <c r="E30">
+      <c r="H38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M38" s="1"/>
+    </row>
+    <row r="39" spans="1:13" ht="16" thickTop="1">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39">
+        <v>40</v>
+      </c>
+      <c r="C39" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F30">
+      <c r="F39">
         <f>615.7*60</f>
         <v>36942</v>
       </c>
-      <c r="H30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30">
-        <v>4</v>
-      </c>
-      <c r="J30" s="7">
-        <v>4</v>
-      </c>
-      <c r="K30">
+      <c r="H39" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39">
+        <v>4</v>
+      </c>
+      <c r="J39" s="7">
+        <v>4</v>
+      </c>
+      <c r="K39">
         <v>1</v>
       </c>
-      <c r="L30">
-        <v>4</v>
-      </c>
-      <c r="M30" s="5"/>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31">
+      <c r="L39">
+        <v>4</v>
+      </c>
+      <c r="M39" s="5"/>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40">
         <v>40</v>
       </c>
-      <c r="C31" t="s">
-        <v>3</v>
-      </c>
-      <c r="D31">
+      <c r="C40" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="D40">
         <v>8</v>
       </c>
-      <c r="E31">
+      <c r="E40">
         <v>1.2</v>
       </c>
-      <c r="F31">
+      <c r="F40">
         <v>19618</v>
       </c>
-      <c r="H31" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31">
+      <c r="H40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40">
         <v>2</v>
       </c>
-      <c r="J31" s="7">
-        <v>4</v>
-      </c>
-      <c r="K31">
+      <c r="J40" s="7">
+        <v>4</v>
+      </c>
+      <c r="K40">
         <v>2</v>
       </c>
-      <c r="L31">
+      <c r="L40">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
-      <c r="A32" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32">
+    <row r="41" spans="1:13">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41">
         <v>40</v>
       </c>
-      <c r="C32" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32">
+      <c r="C41" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="D41">
         <v>16</v>
       </c>
-      <c r="E32">
+      <c r="E41">
         <v>0.73199999999999998</v>
       </c>
-      <c r="F32">
+      <c r="F41">
         <v>28299</v>
       </c>
-      <c r="H32" t="s">
-        <v>17</v>
-      </c>
-      <c r="I32">
+      <c r="H41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41">
         <v>1</v>
       </c>
-      <c r="J32" s="7">
-        <v>4</v>
-      </c>
-      <c r="K32">
-        <v>4</v>
-      </c>
-      <c r="L32">
+      <c r="J41" s="7">
+        <v>4</v>
+      </c>
+      <c r="K41">
+        <v>4</v>
+      </c>
+      <c r="L41">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="14" customHeight="1">
-      <c r="A33" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33">
-        <v>40</v>
-      </c>
-      <c r="C33" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33">
-        <v>16</v>
-      </c>
-      <c r="E33">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="F33">
-        <v>25215</v>
-      </c>
-      <c r="H33" t="s">
-        <v>17</v>
-      </c>
-      <c r="I33">
-        <v>4</v>
-      </c>
-      <c r="J33" s="7">
-        <v>4</v>
-      </c>
-      <c r="K33">
-        <v>4</v>
-      </c>
-      <c r="L33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15">
-      <c r="E35" s="3"/>
-    </row>
-    <row r="40" spans="1:15" ht="20" thickBot="1">
-      <c r="A40" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="50" thickTop="1" thickBot="1">
-      <c r="A41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J41" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K41" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M41" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="N41" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O41" s="2"/>
-    </row>
-    <row r="42" spans="1:15" ht="31" thickTop="1">
+    <row r="42" spans="1:13" ht="14" customHeight="1">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B42">
         <v>40</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="D42">
+        <v>16</v>
+      </c>
+      <c r="E42">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="F42">
+        <v>25215</v>
+      </c>
+      <c r="H42" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42">
+        <v>4</v>
+      </c>
+      <c r="J42" s="7">
+        <v>4</v>
+      </c>
+      <c r="K42">
+        <v>4</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="E44" s="3"/>
+    </row>
+    <row r="49" spans="1:15" ht="20" thickBot="1">
+      <c r="A49" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="50" thickTop="1" thickBot="1">
+      <c r="A50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D42">
+      <c r="H50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K50" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="N50" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O50" s="2"/>
+    </row>
+    <row r="51" spans="1:15" ht="31" thickTop="1">
+      <c r="A51" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51">
         <v>40</v>
       </c>
-      <c r="E42">
+      <c r="C51">
+        <v>1.9</v>
+      </c>
+      <c r="D51">
+        <v>40</v>
+      </c>
+      <c r="E51">
         <v>0.20899999999999999</v>
       </c>
-      <c r="F42" s="12"/>
-      <c r="G42">
+      <c r="G51">
         <v>3966</v>
       </c>
-      <c r="H42" t="s">
-        <v>52</v>
-      </c>
-      <c r="I42">
+      <c r="H51" t="s">
+        <v>50</v>
+      </c>
+      <c r="I51">
         <v>2</v>
       </c>
-      <c r="J42" s="7">
+      <c r="J51" s="7">
         <v>80</v>
       </c>
-      <c r="K42" s="8">
+      <c r="K51" s="8">
         <v>10</v>
       </c>
-      <c r="L42">
+      <c r="L51">
         <v>2</v>
       </c>
-      <c r="M42">
+      <c r="M51">
         <v>105</v>
       </c>
-      <c r="N42" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15">
-      <c r="A43" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43">
+      <c r="N51" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52">
         <v>40</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C52">
+        <v>1.9</v>
+      </c>
+      <c r="D52">
+        <v>20</v>
+      </c>
+      <c r="E52">
+        <v>0.435</v>
+      </c>
+      <c r="G52">
+        <v>8031</v>
+      </c>
+      <c r="H52" t="s">
+        <v>50</v>
+      </c>
+      <c r="I52">
+        <v>2</v>
+      </c>
+      <c r="J52" s="7">
+        <v>40</v>
+      </c>
+      <c r="K52" s="7">
+        <v>5</v>
+      </c>
+      <c r="L52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
+      <c r="A53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53">
+        <v>40</v>
+      </c>
+      <c r="C53">
+        <v>1.9</v>
+      </c>
+      <c r="D53">
+        <v>40</v>
+      </c>
+      <c r="E53">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="G53">
+        <v>25807</v>
+      </c>
+      <c r="H53" t="s">
+        <v>5</v>
+      </c>
+      <c r="I53">
+        <v>2</v>
+      </c>
+      <c r="J53" s="7">
+        <v>12</v>
+      </c>
+      <c r="K53" s="8">
         <v>3</v>
       </c>
-      <c r="D43">
+      <c r="L53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
+      <c r="A54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54">
+        <v>40</v>
+      </c>
+      <c r="C54">
+        <v>1.9</v>
+      </c>
+      <c r="D54">
         <v>20</v>
       </c>
-      <c r="E43">
+      <c r="E54">
         <v>0.435</v>
       </c>
-      <c r="F43" s="13"/>
-      <c r="G43">
-        <v>8031</v>
-      </c>
-      <c r="H43" t="s">
-        <v>52</v>
-      </c>
-      <c r="I43">
+      <c r="G54">
+        <v>23872</v>
+      </c>
+      <c r="H54" t="s">
+        <v>5</v>
+      </c>
+      <c r="I54">
         <v>2</v>
       </c>
-      <c r="J43" s="7">
+      <c r="J54" s="7">
+        <v>12</v>
+      </c>
+      <c r="K54" s="7">
+        <v>3</v>
+      </c>
+      <c r="L54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
+      <c r="A55" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55">
         <v>40</v>
       </c>
-      <c r="K43" s="7">
-        <v>5</v>
-      </c>
-      <c r="L43">
+      <c r="C55">
+        <v>1.9</v>
+      </c>
+      <c r="D55">
+        <v>40</v>
+      </c>
+      <c r="E55">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="H55" t="s">
+        <v>50</v>
+      </c>
+      <c r="I55">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:15">
-      <c r="A44" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44">
+      <c r="J55" s="7">
+        <v>16</v>
+      </c>
+      <c r="K55" s="8">
+        <v>2</v>
+      </c>
+      <c r="L55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56">
         <v>40</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C56">
+        <v>1.9</v>
+      </c>
+      <c r="D56">
+        <v>20</v>
+      </c>
+      <c r="E56">
+        <v>0.435</v>
+      </c>
+      <c r="H56" t="s">
+        <v>50</v>
+      </c>
+      <c r="I56">
+        <v>2</v>
+      </c>
+      <c r="J56" s="7">
+        <v>16</v>
+      </c>
+      <c r="K56" s="7">
+        <v>2</v>
+      </c>
+      <c r="L56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
+      <c r="E57" s="3"/>
+    </row>
+    <row r="61" spans="1:15">
+      <c r="J61" s="7"/>
+      <c r="K61" s="7"/>
+    </row>
+    <row r="62" spans="1:15">
+      <c r="K62" s="7"/>
+    </row>
+    <row r="63" spans="1:15" ht="20" thickBot="1">
+      <c r="A63" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K63" s="7"/>
+    </row>
+    <row r="64" spans="1:15" ht="50" thickTop="1" thickBot="1">
+      <c r="A64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D44">
-        <v>40</v>
-      </c>
-      <c r="E44">
-        <v>0.20899999999999999</v>
-      </c>
-      <c r="F44" s="12"/>
-      <c r="G44">
-        <v>25807</v>
-      </c>
-      <c r="H44" t="s">
+      <c r="H64" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J64" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K64" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M64" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N64" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="16" thickTop="1">
+      <c r="A65" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="I44">
-        <v>2</v>
-      </c>
-      <c r="J44" s="7">
-        <v>12</v>
-      </c>
-      <c r="K44" s="8">
-        <v>3</v>
-      </c>
-      <c r="L44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15">
-      <c r="A45" t="s">
-        <v>7</v>
-      </c>
-      <c r="B45">
-        <v>40</v>
-      </c>
-      <c r="C45" t="s">
-        <v>3</v>
-      </c>
-      <c r="D45">
-        <v>20</v>
-      </c>
-      <c r="E45">
-        <v>0.435</v>
-      </c>
-      <c r="F45" s="13"/>
-      <c r="G45">
-        <v>23872</v>
-      </c>
-      <c r="H45" t="s">
-        <v>6</v>
-      </c>
-      <c r="I45">
-        <v>2</v>
-      </c>
-      <c r="J45" s="7">
-        <v>12</v>
-      </c>
-      <c r="K45" s="7">
-        <v>3</v>
-      </c>
-      <c r="L45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15">
-      <c r="A46" t="s">
-        <v>7</v>
-      </c>
-      <c r="B46">
-        <v>40</v>
-      </c>
-      <c r="C46" t="s">
-        <v>3</v>
-      </c>
-      <c r="D46">
-        <v>40</v>
-      </c>
-      <c r="E46">
-        <v>0.20899999999999999</v>
-      </c>
-      <c r="F46" s="12"/>
-      <c r="H46" t="s">
-        <v>52</v>
-      </c>
-      <c r="I46">
-        <v>2</v>
-      </c>
-      <c r="J46" s="7">
-        <v>16</v>
-      </c>
-      <c r="K46" s="8">
-        <v>2</v>
-      </c>
-      <c r="L46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15">
-      <c r="A47" t="s">
-        <v>7</v>
-      </c>
-      <c r="B47">
-        <v>40</v>
-      </c>
-      <c r="C47" t="s">
-        <v>3</v>
-      </c>
-      <c r="D47">
-        <v>20</v>
-      </c>
-      <c r="E47">
-        <v>0.435</v>
-      </c>
-      <c r="F47" s="13"/>
-      <c r="H47" t="s">
-        <v>52</v>
-      </c>
-      <c r="I47">
-        <v>2</v>
-      </c>
-      <c r="J47" s="7">
-        <v>16</v>
-      </c>
-      <c r="K47" s="7">
-        <v>2</v>
-      </c>
-      <c r="L47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15">
-      <c r="E48" s="3"/>
-    </row>
-    <row r="52" spans="1:14">
-      <c r="F52" s="13"/>
-      <c r="J52" s="7"/>
-      <c r="K52" s="7"/>
-    </row>
-    <row r="53" spans="1:14">
-      <c r="F53" s="13"/>
-      <c r="K53" s="7"/>
-    </row>
-    <row r="54" spans="1:14" ht="20" thickBot="1">
-      <c r="A54" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F54" s="13"/>
-      <c r="K54" s="7"/>
-    </row>
-    <row r="55" spans="1:14" ht="50" thickTop="1" thickBot="1">
-      <c r="A55" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F55" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J55" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K55" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L55" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M55" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N55" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" ht="16" thickTop="1">
-      <c r="A56" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B56" s="7">
-        <v>40</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D56" s="7">
-        <v>40</v>
-      </c>
-      <c r="E56" s="7">
-        <v>0.20899999999999999</v>
-      </c>
-      <c r="F56" s="12"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I56" s="7">
-        <v>2</v>
-      </c>
-      <c r="J56" s="7">
-        <v>80</v>
-      </c>
-      <c r="K56" s="8">
-        <v>0</v>
-      </c>
-      <c r="L56" s="7">
-        <v>2</v>
-      </c>
-      <c r="M56" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14">
-      <c r="A57" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B57" s="7">
-        <v>40</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D57" s="7">
-        <v>20</v>
-      </c>
-      <c r="E57" s="7">
-        <v>0.435</v>
-      </c>
-      <c r="F57" s="12"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I57" s="7">
-        <v>2</v>
-      </c>
-      <c r="J57" s="7">
-        <v>40</v>
-      </c>
-      <c r="K57" s="7">
-        <v>0</v>
-      </c>
-      <c r="L57" s="7">
-        <v>2</v>
-      </c>
-      <c r="M57" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14">
-      <c r="F58" s="12"/>
-    </row>
-    <row r="59" spans="1:14">
-      <c r="F59" s="12"/>
-    </row>
-    <row r="60" spans="1:14">
-      <c r="F60" s="12"/>
-    </row>
-    <row r="61" spans="1:14">
-      <c r="F61" s="12"/>
-    </row>
-    <row r="62" spans="1:14" ht="20" thickBot="1">
-      <c r="A62" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F62" s="12"/>
-    </row>
-    <row r="63" spans="1:14" ht="50" thickTop="1" thickBot="1">
-      <c r="A63" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F63" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J63" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K63" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L63" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M63" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" ht="16" thickTop="1">
-      <c r="A64" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B64" s="7">
-        <v>40</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D64" s="7">
-        <v>40</v>
-      </c>
-      <c r="E64" s="7">
-        <v>0.20899999999999999</v>
-      </c>
-      <c r="F64" s="12"/>
-      <c r="G64" s="7"/>
-      <c r="H64" t="s">
-        <v>45</v>
-      </c>
-      <c r="I64" s="7">
-        <v>2</v>
-      </c>
-      <c r="J64" s="7">
-        <v>80</v>
-      </c>
-      <c r="K64" s="7">
-        <v>10</v>
-      </c>
-      <c r="M64" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13">
-      <c r="A65" s="7" t="s">
-        <v>7</v>
       </c>
       <c r="B65" s="7">
         <v>40</v>
       </c>
-      <c r="C65" s="7" t="s">
-        <v>3</v>
+      <c r="C65">
+        <v>1.9</v>
       </c>
       <c r="D65" s="7">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E65" s="7">
-        <v>0.435</v>
-      </c>
-      <c r="F65" s="12"/>
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="F65" s="7">
+        <v>3468</v>
+      </c>
       <c r="G65" s="7"/>
-      <c r="H65" t="s">
-        <v>45</v>
+      <c r="H65" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="I65" s="7">
         <v>2</v>
@@ -3160,110 +3099,262 @@
       <c r="J65" s="7">
         <v>80</v>
       </c>
-      <c r="K65" s="7">
-        <v>6</v>
+      <c r="K65" s="8">
+        <v>0</v>
+      </c>
+      <c r="L65" s="7">
+        <v>2</v>
       </c>
       <c r="M65" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="45">
-      <c r="A74" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="M74" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13">
-      <c r="K75">
+    <row r="66" spans="1:13">
+      <c r="A66" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" s="7">
+        <v>40</v>
+      </c>
+      <c r="C66">
+        <v>1.9</v>
+      </c>
+      <c r="D66" s="7">
+        <v>20</v>
+      </c>
+      <c r="E66" s="7">
+        <v>0.435</v>
+      </c>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I66" s="7">
+        <v>2</v>
+      </c>
+      <c r="J66" s="7">
+        <v>40</v>
+      </c>
+      <c r="K66" s="7">
+        <v>0</v>
+      </c>
+      <c r="L66" s="7">
+        <v>2</v>
+      </c>
+      <c r="M66" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="20" thickBot="1">
+      <c r="A71" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="50" thickTop="1" thickBot="1">
+      <c r="A72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L75" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13">
-      <c r="K76" s="3">
+      <c r="C72" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L76" s="3"/>
-      <c r="M76">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13">
-      <c r="A77" s="9" t="s">
+      <c r="E72" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J72" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K72" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L72" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M72" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="16" thickTop="1">
+      <c r="A73" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" s="7">
+        <v>40</v>
+      </c>
+      <c r="C73">
+        <v>1.9</v>
+      </c>
+      <c r="D73" s="7">
+        <v>40</v>
+      </c>
+      <c r="E73" s="7">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="G73" s="7"/>
+      <c r="H73" t="s">
+        <v>44</v>
+      </c>
+      <c r="I73" s="7">
+        <v>2</v>
+      </c>
+      <c r="J73" s="7">
+        <v>80</v>
+      </c>
+      <c r="K73" s="7">
+        <v>10</v>
+      </c>
+      <c r="M73" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13">
+      <c r="A74" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74" s="7">
+        <v>40</v>
+      </c>
+      <c r="C74">
+        <v>1.9</v>
+      </c>
+      <c r="D74" s="7">
+        <v>20</v>
+      </c>
+      <c r="E74" s="7">
+        <v>0.435</v>
+      </c>
+      <c r="G74" s="7"/>
+      <c r="H74" t="s">
+        <v>44</v>
+      </c>
+      <c r="I74" s="7">
+        <v>2</v>
+      </c>
+      <c r="J74" s="7">
+        <v>80</v>
+      </c>
+      <c r="K74" s="7">
+        <v>6</v>
+      </c>
+      <c r="M74" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" ht="45">
+      <c r="A83" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="M83" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13">
+      <c r="K84">
+        <v>1</v>
+      </c>
+      <c r="L84" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13">
+      <c r="K85" s="3">
+        <v>2</v>
+      </c>
+      <c r="L85" s="3"/>
+      <c r="M85">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13">
+      <c r="A86" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13">
+      <c r="A87" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13">
+      <c r="A88" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:13">
-      <c r="A78" s="9" t="s">
+    <row r="89" spans="1:13">
+      <c r="A89" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13">
+      <c r="A90" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13">
+      <c r="A91" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13">
+      <c r="A92" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:13">
-      <c r="A79" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13">
-      <c r="A80" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1">
-      <c r="A81" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1">
-      <c r="A82" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1">
-      <c r="A83" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1">
-      <c r="A89" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1">
-      <c r="A90" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91" s="9" t="s">
+    <row r="101" spans="1:1">
+      <c r="A101" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
-      <c r="A92" s="9" t="s">
+    <row r="102" spans="1:1">
+      <c r="A102" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
-      <c r="A93" s="9" t="s">
+    <row r="103" spans="1:1">
+      <c r="A103" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
-      <c r="A94" s="9" t="s">
+    <row r="104" spans="1:1">
+      <c r="A104" s="9" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1">
-      <c r="A95" s="9" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
adding new template, diskspace table
git-svn-id: file://localhost/tmp/svn2git/svn@3762 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/data-intensive-bio/Results.xlsx
+++ b/papers/data-intensive-bio/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="129"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28560" windowHeight="17280" tabRatio="129"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -374,7 +374,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="260">
+  <cellStyleXfs count="268">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -455,6 +455,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -669,7 +677,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="260">
+  <cellStyles count="268">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -798,6 +806,10 @@
     <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="10" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
@@ -928,6 +940,10 @@
     <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="258" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="260" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Warning Text" xfId="79" builtinId="11"/>
   </cellStyles>
@@ -1147,11 +1163,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="504618952"/>
-        <c:axId val="603506072"/>
+        <c:axId val="543676328"/>
+        <c:axId val="543197992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="504618952"/>
+        <c:axId val="543676328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1180,12 +1196,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="603506072"/>
+        <c:crossAx val="543197992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="603506072"/>
+        <c:axId val="543197992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1219,7 +1235,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="504618952"/>
+        <c:crossAx val="543676328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1505,11 +1521,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="603321160"/>
-        <c:axId val="603326296"/>
+        <c:axId val="500702520"/>
+        <c:axId val="3212168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="603321160"/>
+        <c:axId val="500702520"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -1539,12 +1555,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="603326296"/>
+        <c:crossAx val="3212168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="603326296"/>
+        <c:axId val="3212168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1573,7 +1589,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="603321160"/>
+        <c:crossAx val="500702520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1727,11 +1743,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="603495496"/>
-        <c:axId val="603574664"/>
+        <c:axId val="543731560"/>
+        <c:axId val="500662824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="603495496"/>
+        <c:axId val="543731560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1741,13 +1757,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="603574664"/>
+        <c:crossAx val="500662824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="603574664"/>
+        <c:axId val="500662824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1757,7 +1773,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="603495496"/>
+        <c:crossAx val="543731560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2193,8 +2209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
-      <selection activeCell="G77" sqref="G77"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3684,7 +3700,7 @@
         <v>40</v>
       </c>
       <c r="E70" s="7">
-        <v>0.22900000000000001</v>
+        <v>1</v>
       </c>
       <c r="F70" s="7">
         <v>3468</v>
@@ -3765,7 +3781,7 @@
         <v>907</v>
       </c>
       <c r="G72" s="7">
-        <v>980</v>
+        <v>1020</v>
       </c>
       <c r="H72" s="7" t="s">
         <v>74</v>
@@ -4443,6 +4459,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
new data from ranger
git-svn-id: file://localhost/tmp/svn2git/svn@4019 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/data-intensive-bio/Results.xlsx
+++ b/papers/data-intensive-bio/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="0" windowWidth="25600" windowHeight="15620" tabRatio="211"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15920" tabRatio="211" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ranger" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="100">
   <si>
     <t>Type</t>
   </si>
@@ -280,9 +280,6 @@
     <t>Human Genome(hg18)</t>
   </si>
   <si>
-    <t>Time For  Match  files(sec)</t>
-  </si>
-  <si>
     <t>Prepare Read files step</t>
   </si>
   <si>
@@ -314,6 +311,15 @@
   </si>
   <si>
     <t>all jobs are concurrent</t>
+  </si>
+  <si>
+    <t>Time (sec)</t>
+  </si>
+  <si>
+    <t>Time(sec)</t>
+  </si>
+  <si>
+    <t>Ranger 16 core , RAM 32GB</t>
   </si>
 </sst>
 </file>
@@ -444,7 +450,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="350">
+  <cellStyleXfs count="360">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -525,6 +531,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -831,7 +847,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="350">
+  <cellStyles count="360">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1005,6 +1021,11 @@
     <cellStyle name="Followed Hyperlink" xfId="345" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="347" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="349" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="351" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="353" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="355" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="357" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="359" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="10" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
@@ -1180,6 +1201,11 @@
     <cellStyle name="Hyperlink" xfId="344" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="346" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="348" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="350" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="352" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="354" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="356" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="358" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Warning Text" xfId="79" builtinId="11"/>
   </cellStyles>
@@ -1215,7 +1241,7 @@
               <a:rPr lang="en-US" sz="1200" b="0" i="0">
                 <a:latin typeface="Times New Roman"/>
               </a:rPr>
-              <a:t>Number of read files vs</a:t>
+              <a:t>Size of read files vs</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
@@ -1349,7 +1375,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>OLd_data!$E$32:$E$35</c:f>
+              <c:f>OLd_data!$E$34:$E$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1370,7 +1396,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>OLd_data!$F$32:$F$35</c:f>
+              <c:f>OLd_data!$F$34:$F$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1445,6 +1471,9 @@
                 <c:pt idx="4">
                   <c:v>7663.0</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>15001.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1512,6 +1541,56 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Ranger 10 index files</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>OLd_data!$E$24:$E$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.435</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>OLd_data!$F$24:$F$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>23287.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12364.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7042.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5526.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1520,11 +1599,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="388076696"/>
-        <c:axId val="485122952"/>
+        <c:axId val="551875080"/>
+        <c:axId val="551882024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="388076696"/>
+        <c:axId val="551875080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1553,12 +1632,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="485122952"/>
+        <c:crossAx val="551882024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="485122952"/>
+        <c:axId val="551882024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1592,7 +1671,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="388076696"/>
+        <c:crossAx val="551875080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1611,8 +1690,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.80453177727784"/>
           <c:y val="0.334909377635167"/>
-          <c:w val="0.195468211101711"/>
-          <c:h val="0.198594940774554"/>
+          <c:w val="0.194127243066884"/>
+          <c:h val="0.223391695059252"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1670,6 +1749,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1715,7 +1795,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>OLd_data!$I$42:$I$48</c:f>
+              <c:f>OLd_data!$I$44:$I$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1745,7 +1825,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>OLd_data!$F$42:$F$48</c:f>
+              <c:f>OLd_data!$F$44:$F$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1783,7 +1863,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>OLd_data!$I$50:$I$53</c:f>
+              <c:f>OLd_data!$I$52:$I$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1804,7 +1884,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>OLd_data!$F$50:$F$53</c:f>
+              <c:f>OLd_data!$F$52:$F$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1833,7 +1913,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>OLd_data!$I$55:$I$57</c:f>
+              <c:f>OLd_data!$I$57:$I$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1851,7 +1931,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>OLd_data!$F$55:$F$57</c:f>
+              <c:f>OLd_data!$F$57:$F$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1877,11 +1957,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="484747336"/>
-        <c:axId val="484719672"/>
+        <c:axId val="551949768"/>
+        <c:axId val="551955272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="484747336"/>
+        <c:axId val="551949768"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -1904,18 +1984,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="484719672"/>
+        <c:crossAx val="551955272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="484719672"/>
+        <c:axId val="551955272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1937,13 +2018,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="484747336"/>
+        <c:crossAx val="551949768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2053,7 +2135,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>OLd_data!$K$62:$K$64</c:f>
+              <c:f>OLd_data!$K$64:$K$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2071,7 +2153,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>OLd_data!$F$62:$F$64</c:f>
+              <c:f>OLd_data!$F$64:$F$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2097,11 +2179,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="383343224"/>
-        <c:axId val="485230280"/>
+        <c:axId val="551980184"/>
+        <c:axId val="551984664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="383343224"/>
+        <c:axId val="551980184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2111,13 +2193,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="485230280"/>
+        <c:crossAx val="551984664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="485230280"/>
+        <c:axId val="551984664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2127,7 +2209,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="383343224"/>
+        <c:crossAx val="551980184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2149,15 +2231,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>889000</xdr:colOff>
+      <xdr:colOff>520700</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2180,13 +2262,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>863600</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>508000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2563,27 +2645,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20" thickBot="1">
       <c r="A1" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="16" thickTop="1"/>
     <row r="3" spans="1:9" ht="20" thickBot="1">
       <c r="A3" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="50" thickTop="1" thickBot="1">
@@ -2591,10 +2673,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>4</v>
@@ -2606,7 +2688,7 @@
         <v>18</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16" thickTop="1">
@@ -2651,13 +2733,13 @@
     </row>
     <row r="10" spans="1:9" ht="20" thickBot="1">
       <c r="A10" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="50" thickTop="1" thickBot="1">
@@ -2674,19 +2756,19 @@
         <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="16" thickTop="1">
@@ -2750,13 +2832,13 @@
     </row>
     <row r="16" spans="1:9" ht="20" thickBot="1">
       <c r="A16" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="50" thickTop="1" thickBot="1">
@@ -2773,16 +2855,16 @@
         <v>4</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>22</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="16" thickTop="1">
@@ -2844,10 +2926,10 @@
         <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="50" thickTop="1" thickBot="1">
@@ -2864,16 +2946,16 @@
         <v>4</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>22</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="16" thickTop="1">
@@ -2931,7 +3013,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2942,10 +3023,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O206"/>
+  <dimension ref="A1:O208"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2956,7 +3037,7 @@
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" customWidth="1"/>
     <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
     <col min="8" max="8" width="12.83203125" customWidth="1"/>
     <col min="9" max="9" width="22.5" customWidth="1"/>
     <col min="10" max="10" width="14.1640625" customWidth="1"/>
@@ -2983,6 +3064,9 @@
       <c r="F1" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="2" spans="1:12" ht="60" customHeight="1" thickTop="1" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -3329,6 +3413,9 @@
       <c r="E13">
         <v>2</v>
       </c>
+      <c r="F13">
+        <v>15001</v>
+      </c>
       <c r="H13" t="s">
         <v>55</v>
       </c>
@@ -3547,22 +3634,25 @@
         <v>40</v>
       </c>
       <c r="C24">
-        <v>1.9</v>
+        <v>129</v>
       </c>
       <c r="D24">
         <v>4</v>
       </c>
       <c r="E24">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
+      </c>
+      <c r="F24">
+        <v>23287</v>
       </c>
       <c r="H24" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="I24">
-        <v>4</v>
-      </c>
-      <c r="J24" s="7">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="J24">
+        <v>16</v>
       </c>
       <c r="K24" s="7">
         <v>1</v>
@@ -3576,7 +3666,7 @@
         <v>40</v>
       </c>
       <c r="C25">
-        <v>1.9</v>
+        <v>129</v>
       </c>
       <c r="D25">
         <v>8</v>
@@ -3584,14 +3674,17 @@
       <c r="E25">
         <v>1.2</v>
       </c>
+      <c r="F25">
+        <v>12364</v>
+      </c>
       <c r="H25" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="I25">
-        <v>4</v>
-      </c>
-      <c r="J25" s="7">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="J25">
+        <v>16</v>
       </c>
       <c r="K25" s="7">
         <v>1</v>
@@ -3605,22 +3698,25 @@
         <v>40</v>
       </c>
       <c r="C26">
-        <v>1.9</v>
+        <v>129</v>
       </c>
       <c r="D26">
         <v>12</v>
       </c>
       <c r="E26">
-        <v>0.73199999999999998</v>
+        <v>0.6</v>
+      </c>
+      <c r="F26">
+        <v>7042</v>
       </c>
       <c r="H26" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="I26">
-        <v>4</v>
-      </c>
-      <c r="J26" s="7">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="J26">
+        <v>16</v>
       </c>
       <c r="K26" s="7">
         <v>1</v>
@@ -3634,146 +3730,85 @@
         <v>40</v>
       </c>
       <c r="C27">
-        <v>1.9</v>
+        <v>129</v>
       </c>
       <c r="D27">
         <v>37</v>
       </c>
       <c r="E27">
-        <v>0.22900000000000001</v>
+        <v>0.435</v>
+      </c>
+      <c r="F27">
+        <v>5526</v>
       </c>
       <c r="H27" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="I27">
+        <v>16</v>
+      </c>
+      <c r="J27">
+        <v>16</v>
+      </c>
+      <c r="K27" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="H30" s="7"/>
+    </row>
+    <row r="32" spans="1:15" ht="20" thickBot="1">
+      <c r="A32" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="50" thickTop="1" thickBot="1">
+      <c r="A33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J27" s="7">
-        <v>4</v>
-      </c>
-      <c r="K27" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15">
-      <c r="H28" s="7"/>
-    </row>
-    <row r="30" spans="1:15" ht="20" thickBot="1">
-      <c r="A30" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="50" thickTop="1" thickBot="1">
-      <c r="A31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I31" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J31" s="6" t="s">
+      <c r="J33" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K31" s="6" t="s">
+      <c r="K33" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L31" s="2" t="s">
+      <c r="L33" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="16" thickTop="1">
-      <c r="A32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32">
-        <v>10</v>
-      </c>
-      <c r="C32">
-        <v>1.7</v>
-      </c>
-      <c r="D32">
-        <v>4</v>
-      </c>
-      <c r="E32">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F32" s="13">
-        <v>8810</v>
-      </c>
-      <c r="H32" t="s">
-        <v>12</v>
-      </c>
-      <c r="I32">
-        <v>4</v>
-      </c>
-      <c r="J32" s="7">
-        <v>4</v>
-      </c>
-      <c r="K32" s="8">
-        <v>1</v>
-      </c>
-      <c r="L32">
-        <f>D32*F32</f>
-        <v>35240</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12">
-      <c r="A33" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33">
-        <v>10</v>
-      </c>
-      <c r="C33">
-        <v>1.7</v>
-      </c>
-      <c r="D33">
-        <v>8</v>
-      </c>
-      <c r="E33">
-        <v>1.2</v>
-      </c>
-      <c r="F33" s="13">
-        <v>4428</v>
-      </c>
-      <c r="H33" t="s">
-        <v>12</v>
-      </c>
-      <c r="I33">
-        <v>4</v>
-      </c>
-      <c r="J33" s="7">
-        <v>4</v>
-      </c>
-      <c r="K33" s="7">
-        <v>1</v>
-      </c>
-      <c r="L33">
-        <f>D33*F33</f>
-        <v>35424</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" ht="16" thickTop="1">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -3784,13 +3819,13 @@
         <v>1.7</v>
       </c>
       <c r="D34">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E34">
-        <v>0.73199999999999998</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F34" s="13">
-        <v>2855</v>
+        <v>8810</v>
       </c>
       <c r="H34" t="s">
         <v>12</v>
@@ -3801,38 +3836,37 @@
       <c r="J34" s="7">
         <v>4</v>
       </c>
-      <c r="K34" s="7">
+      <c r="K34" s="8">
         <v>1</v>
       </c>
       <c r="L34">
         <f>D34*F34</f>
-        <v>34260</v>
+        <v>35240</v>
       </c>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="7" t="s">
+      <c r="A35" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="7">
+      <c r="B35">
         <v>10</v>
       </c>
       <c r="C35">
         <v>1.7</v>
       </c>
-      <c r="D35" s="7">
-        <v>37</v>
-      </c>
-      <c r="E35" s="7">
-        <v>0.22900000000000001</v>
-      </c>
-      <c r="F35" s="14">
-        <v>936</v>
-      </c>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I35" s="7">
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="E35">
+        <v>1.2</v>
+      </c>
+      <c r="F35" s="13">
+        <v>4428</v>
+      </c>
+      <c r="H35" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35">
         <v>4</v>
       </c>
       <c r="J35" s="7">
@@ -3841,38 +3875,45 @@
       <c r="K35" s="7">
         <v>1</v>
       </c>
+      <c r="L35">
+        <f>D35*F35</f>
+        <v>35424</v>
+      </c>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="7" t="s">
+      <c r="A36" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36">
         <v>10</v>
       </c>
       <c r="C36">
         <v>1.7</v>
       </c>
-      <c r="D36" s="7">
-        <v>37</v>
-      </c>
-      <c r="E36" s="7">
-        <v>0.20899999999999999</v>
-      </c>
-      <c r="F36" s="14">
-        <v>524</v>
-      </c>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="I36" s="7">
-        <v>8</v>
+      <c r="D36">
+        <v>12</v>
+      </c>
+      <c r="E36">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="F36" s="13">
+        <v>2855</v>
+      </c>
+      <c r="H36" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36">
+        <v>4</v>
       </c>
       <c r="J36" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K36" s="7">
         <v>1</v>
+      </c>
+      <c r="L36">
+        <f>D36*F36</f>
+        <v>34260</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -3889,20 +3930,20 @@
         <v>37</v>
       </c>
       <c r="E37" s="7">
-        <v>0.20899999999999999</v>
+        <v>0.22900000000000001</v>
       </c>
       <c r="F37" s="14">
-        <v>524</v>
+        <v>936</v>
       </c>
       <c r="G37" s="7"/>
       <c r="H37" s="7" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="I37" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J37" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K37" s="7">
         <v>1</v>
@@ -3922,10 +3963,10 @@
         <v>37</v>
       </c>
       <c r="E38" s="7">
-        <v>0.435</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="F38" s="14">
-        <v>1060</v>
+        <v>524</v>
       </c>
       <c r="G38" s="7"/>
       <c r="H38" s="7" t="s">
@@ -3941,111 +3982,113 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="20" thickBot="1">
-      <c r="A40" s="4" t="s">
+    <row r="39" spans="1:12">
+      <c r="A39" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" ht="66" thickTop="1" thickBot="1">
-      <c r="A41" s="1" t="s">
+      <c r="C39">
+        <v>1.7</v>
+      </c>
+      <c r="D39" s="7">
+        <v>37</v>
+      </c>
+      <c r="E39" s="7">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="F39" s="14">
+        <v>524</v>
+      </c>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="I39" s="7">
+        <v>8</v>
+      </c>
+      <c r="J39" s="7">
+        <v>8</v>
+      </c>
+      <c r="K39" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="7">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <v>1.7</v>
+      </c>
+      <c r="D40" s="7">
+        <v>37</v>
+      </c>
+      <c r="E40" s="7">
+        <v>0.435</v>
+      </c>
+      <c r="F40" s="14">
+        <v>1060</v>
+      </c>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="I40" s="7">
+        <v>8</v>
+      </c>
+      <c r="J40" s="7">
+        <v>8</v>
+      </c>
+      <c r="K40" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="20" thickBot="1">
+      <c r="A42" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="66" thickTop="1" thickBot="1">
+      <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41" s="6" t="s">
+      <c r="B43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I41" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J41" s="6" t="s">
+      <c r="J43" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K41" s="6" t="s">
+      <c r="K43" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="16" thickTop="1">
-      <c r="A42" t="s">
-        <v>6</v>
-      </c>
-      <c r="B42">
-        <v>40</v>
-      </c>
-      <c r="C42">
-        <v>1.9</v>
-      </c>
-      <c r="D42">
-        <v>37</v>
-      </c>
-      <c r="E42">
-        <v>0.22900000000000001</v>
-      </c>
-      <c r="F42">
-        <v>3539</v>
-      </c>
-      <c r="H42" t="s">
-        <v>7</v>
-      </c>
-      <c r="I42">
-        <v>1</v>
-      </c>
-      <c r="J42" s="7">
-        <v>12</v>
-      </c>
-      <c r="K42" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12">
-      <c r="A43" t="s">
-        <v>6</v>
-      </c>
-      <c r="B43">
-        <v>40</v>
-      </c>
-      <c r="C43">
-        <v>1.9</v>
-      </c>
-      <c r="D43">
-        <v>37</v>
-      </c>
-      <c r="E43">
-        <v>0.22900000000000001</v>
-      </c>
-      <c r="F43">
-        <v>2908</v>
-      </c>
-      <c r="H43" t="s">
-        <v>7</v>
-      </c>
-      <c r="I43">
-        <v>4</v>
-      </c>
-      <c r="J43" s="7">
-        <v>12</v>
-      </c>
-      <c r="K43" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" ht="16" thickTop="1">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -4062,18 +4105,18 @@
         <v>0.22900000000000001</v>
       </c>
       <c r="F44">
-        <v>2834</v>
+        <v>3539</v>
       </c>
       <c r="H44" t="s">
         <v>7</v>
       </c>
       <c r="I44">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="J44" s="7">
         <v>12</v>
       </c>
-      <c r="K44" s="7">
+      <c r="K44" s="8">
         <v>1</v>
       </c>
     </row>
@@ -4094,13 +4137,13 @@
         <v>0.22900000000000001</v>
       </c>
       <c r="F45">
-        <v>2718</v>
+        <v>2908</v>
       </c>
       <c r="H45" t="s">
         <v>7</v>
       </c>
       <c r="I45">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J45" s="7">
         <v>12</v>
@@ -4126,13 +4169,13 @@
         <v>0.22900000000000001</v>
       </c>
       <c r="F46">
-        <v>2716</v>
+        <v>2834</v>
       </c>
       <c r="H46" t="s">
         <v>7</v>
       </c>
       <c r="I46">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="J46" s="7">
         <v>12</v>
@@ -4158,13 +4201,13 @@
         <v>0.22900000000000001</v>
       </c>
       <c r="F47">
-        <v>2725</v>
+        <v>2718</v>
       </c>
       <c r="H47" t="s">
         <v>7</v>
       </c>
       <c r="I47">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="J47" s="7">
         <v>12</v>
@@ -4190,13 +4233,13 @@
         <v>0.22900000000000001</v>
       </c>
       <c r="F48">
-        <v>2715</v>
+        <v>2716</v>
       </c>
       <c r="H48" t="s">
         <v>7</v>
       </c>
       <c r="I48">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="J48" s="7">
         <v>12</v>
@@ -4206,8 +4249,36 @@
       </c>
     </row>
     <row r="49" spans="1:13">
-      <c r="J49" s="7"/>
-      <c r="K49" s="7"/>
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49">
+        <v>40</v>
+      </c>
+      <c r="C49">
+        <v>1.9</v>
+      </c>
+      <c r="D49">
+        <v>37</v>
+      </c>
+      <c r="E49">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="F49">
+        <v>2725</v>
+      </c>
+      <c r="H49" t="s">
+        <v>7</v>
+      </c>
+      <c r="I49">
+        <v>20</v>
+      </c>
+      <c r="J49" s="7">
+        <v>12</v>
+      </c>
+      <c r="K49" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" t="s">
@@ -4220,19 +4291,19 @@
         <v>1.9</v>
       </c>
       <c r="D50">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="E50">
-        <v>1.2</v>
+        <v>0.22900000000000001</v>
       </c>
       <c r="F50">
-        <v>13996</v>
+        <v>2715</v>
       </c>
       <c r="H50" t="s">
         <v>7</v>
       </c>
       <c r="I50">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="J50" s="7">
         <v>12</v>
@@ -4242,36 +4313,8 @@
       </c>
     </row>
     <row r="51" spans="1:13">
-      <c r="A51" t="s">
-        <v>6</v>
-      </c>
-      <c r="B51">
-        <v>40</v>
-      </c>
-      <c r="C51">
-        <v>1.9</v>
-      </c>
-      <c r="D51">
-        <v>8</v>
-      </c>
-      <c r="E51">
-        <v>1.2</v>
-      </c>
-      <c r="F51">
-        <v>13583</v>
-      </c>
-      <c r="H51" t="s">
-        <v>7</v>
-      </c>
-      <c r="I51">
-        <v>8</v>
-      </c>
-      <c r="J51" s="7">
-        <v>12</v>
-      </c>
-      <c r="K51" s="7">
-        <v>1</v>
-      </c>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
     </row>
     <row r="52" spans="1:13">
       <c r="A52" t="s">
@@ -4290,13 +4333,13 @@
         <v>1.2</v>
       </c>
       <c r="F52">
-        <v>12960</v>
+        <v>13996</v>
       </c>
       <c r="H52" t="s">
         <v>7</v>
       </c>
       <c r="I52">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J52" s="7">
         <v>12</v>
@@ -4322,77 +4365,83 @@
         <v>1.2</v>
       </c>
       <c r="F53">
-        <v>12881</v>
+        <v>13583</v>
       </c>
       <c r="H53" t="s">
         <v>7</v>
       </c>
       <c r="I53">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="J53" s="7">
         <v>12</v>
       </c>
       <c r="K53" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54">
+        <v>40</v>
+      </c>
+      <c r="C54">
+        <v>1.9</v>
+      </c>
+      <c r="D54">
+        <v>8</v>
+      </c>
+      <c r="E54">
+        <v>1.2</v>
+      </c>
+      <c r="F54">
+        <v>12960</v>
+      </c>
+      <c r="H54" t="s">
+        <v>7</v>
+      </c>
+      <c r="I54">
+        <v>12</v>
+      </c>
+      <c r="J54" s="7">
+        <v>12</v>
+      </c>
+      <c r="K54" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:13">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="B55">
         <v>40</v>
       </c>
       <c r="C55">
-        <v>0.435</v>
+        <v>1.9</v>
       </c>
       <c r="D55">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="F55">
-        <v>8247</v>
+        <v>12881</v>
       </c>
       <c r="H55" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="I55">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J55" s="7">
         <v>12</v>
       </c>
-    </row>
-    <row r="56" spans="1:13">
-      <c r="A56" t="s">
-        <v>53</v>
-      </c>
-      <c r="B56">
-        <v>40</v>
-      </c>
-      <c r="C56">
-        <v>0.435</v>
-      </c>
-      <c r="D56">
-        <v>5</v>
-      </c>
-      <c r="E56">
-        <v>1</v>
-      </c>
-      <c r="F56">
-        <v>7740</v>
-      </c>
-      <c r="H56" t="s">
-        <v>55</v>
-      </c>
-      <c r="I56">
-        <v>8</v>
-      </c>
-      <c r="J56" s="7">
-        <v>12</v>
+      <c r="K55" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:13">
@@ -4412,173 +4461,161 @@
         <v>1</v>
       </c>
       <c r="F57">
-        <v>7515</v>
+        <v>8247</v>
       </c>
       <c r="H57" t="s">
         <v>55</v>
       </c>
       <c r="I57">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J57" s="7">
         <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:13">
-      <c r="J58" s="7"/>
-    </row>
-    <row r="60" spans="1:13" ht="20" thickBot="1">
-      <c r="A60" s="4" t="s">
+      <c r="A58" t="s">
+        <v>53</v>
+      </c>
+      <c r="B58">
+        <v>40</v>
+      </c>
+      <c r="C58">
+        <v>0.435</v>
+      </c>
+      <c r="D58">
+        <v>5</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>7740</v>
+      </c>
+      <c r="H58" t="s">
+        <v>55</v>
+      </c>
+      <c r="I58">
+        <v>8</v>
+      </c>
+      <c r="J58" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="A59" t="s">
+        <v>53</v>
+      </c>
+      <c r="B59">
+        <v>40</v>
+      </c>
+      <c r="C59">
+        <v>0.435</v>
+      </c>
+      <c r="D59">
+        <v>5</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <v>7515</v>
+      </c>
+      <c r="H59" t="s">
+        <v>55</v>
+      </c>
+      <c r="I59">
+        <v>12</v>
+      </c>
+      <c r="J59" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="J60" s="7"/>
+    </row>
+    <row r="62" spans="1:13" ht="20" thickBot="1">
+      <c r="A62" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="50" thickTop="1" thickBot="1">
-      <c r="A61" s="1" t="s">
+    <row r="63" spans="1:13" ht="50" thickTop="1" thickBot="1">
+      <c r="A63" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" s="6" t="s">
+      <c r="B63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E63" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="F63" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G61" s="1" t="s">
+      <c r="G63" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H61" s="1" t="s">
+      <c r="H63" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I61" s="2" t="s">
+      <c r="I63" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J61" s="6" t="s">
+      <c r="J63" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K61" s="1" t="s">
+      <c r="K63" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L61" s="1" t="s">
+      <c r="L63" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M61" s="1"/>
-    </row>
-    <row r="62" spans="1:13" ht="16" thickTop="1">
-      <c r="A62" t="s">
+      <c r="M63" s="1"/>
+    </row>
+    <row r="64" spans="1:13" ht="16" thickTop="1">
+      <c r="A64" t="s">
         <v>6</v>
       </c>
-      <c r="B62">
-        <v>40</v>
-      </c>
-      <c r="C62" s="7">
+      <c r="B64">
+        <v>40</v>
+      </c>
+      <c r="C64" s="7">
         <v>1.9</v>
       </c>
-      <c r="D62">
+      <c r="D64">
         <v>4</v>
       </c>
-      <c r="E62">
+      <c r="E64">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F62">
+      <c r="F64">
         <f>615.7*60</f>
         <v>36942</v>
       </c>
-      <c r="H62" t="s">
-        <v>15</v>
-      </c>
-      <c r="I62">
-        <v>4</v>
-      </c>
-      <c r="J62" s="7">
-        <v>4</v>
-      </c>
-      <c r="K62">
-        <v>1</v>
-      </c>
-      <c r="L62">
-        <v>4</v>
-      </c>
-      <c r="M62" s="5"/>
-    </row>
-    <row r="63" spans="1:13">
-      <c r="A63" t="s">
-        <v>6</v>
-      </c>
-      <c r="B63">
-        <v>40</v>
-      </c>
-      <c r="C63" s="7">
-        <v>1.9</v>
-      </c>
-      <c r="D63">
-        <v>8</v>
-      </c>
-      <c r="E63">
-        <v>1.2</v>
-      </c>
-      <c r="F63">
-        <v>19618</v>
-      </c>
-      <c r="H63" t="s">
-        <v>15</v>
-      </c>
-      <c r="I63">
-        <v>2</v>
-      </c>
-      <c r="J63" s="7">
-        <v>4</v>
-      </c>
-      <c r="K63">
-        <v>2</v>
-      </c>
-      <c r="L63">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13">
-      <c r="A64" t="s">
-        <v>6</v>
-      </c>
-      <c r="B64">
-        <v>40</v>
-      </c>
-      <c r="C64" s="7">
-        <v>1.9</v>
-      </c>
-      <c r="D64">
-        <v>16</v>
-      </c>
-      <c r="E64">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="F64">
-        <v>28299</v>
-      </c>
       <c r="H64" t="s">
         <v>15</v>
       </c>
       <c r="I64">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J64" s="7">
         <v>4</v>
       </c>
       <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="L64">
         <v>4</v>
       </c>
-      <c r="L64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" ht="14" customHeight="1">
+      <c r="M64" s="5"/>
+    </row>
+    <row r="65" spans="1:12">
       <c r="A65" t="s">
         <v>6</v>
       </c>
@@ -4589,104 +4626,104 @@
         <v>1.9</v>
       </c>
       <c r="D65">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E65">
-        <v>0.73199999999999998</v>
+        <v>1.2</v>
       </c>
       <c r="F65">
-        <v>25215</v>
+        <v>19618</v>
       </c>
       <c r="H65" t="s">
         <v>15</v>
       </c>
       <c r="I65">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J65" s="7">
         <v>4</v>
       </c>
       <c r="K65">
+        <v>2</v>
+      </c>
+      <c r="L65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66">
+        <v>40</v>
+      </c>
+      <c r="C66" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="D66">
+        <v>16</v>
+      </c>
+      <c r="E66">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="F66">
+        <v>28299</v>
+      </c>
+      <c r="H66" t="s">
+        <v>15</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
+      </c>
+      <c r="J66" s="7">
         <v>4</v>
       </c>
-      <c r="L65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15">
-      <c r="E67" s="3"/>
-    </row>
-    <row r="68" spans="1:15">
-      <c r="A68" t="s">
+      <c r="K66">
+        <v>4</v>
+      </c>
+      <c r="L66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="14" customHeight="1">
+      <c r="A67" t="s">
         <v>6</v>
       </c>
-      <c r="B68">
-        <v>10</v>
-      </c>
-      <c r="C68" s="7">
+      <c r="B67">
+        <v>40</v>
+      </c>
+      <c r="C67" s="7">
         <v>1.9</v>
       </c>
-      <c r="D68">
+      <c r="D67">
+        <v>16</v>
+      </c>
+      <c r="E67">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="F67">
+        <v>25215</v>
+      </c>
+      <c r="H67" t="s">
+        <v>15</v>
+      </c>
+      <c r="I67">
         <v>4</v>
       </c>
-      <c r="E68">
-        <v>2.4</v>
-      </c>
-      <c r="F68">
-        <v>9358</v>
-      </c>
-      <c r="H68" t="s">
-        <v>82</v>
-      </c>
-      <c r="I68">
+      <c r="J67" s="7">
         <v>4</v>
       </c>
-      <c r="J68" s="7">
+      <c r="K67">
         <v>4</v>
       </c>
-      <c r="K68">
-        <v>1</v>
-      </c>
-      <c r="L68">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15">
-      <c r="A69" t="s">
-        <v>6</v>
-      </c>
-      <c r="B69">
-        <v>10</v>
-      </c>
-      <c r="C69" s="7">
-        <v>1.9</v>
-      </c>
-      <c r="D69">
-        <v>8</v>
-      </c>
-      <c r="E69">
-        <v>1.2</v>
-      </c>
-      <c r="F69">
-        <v>5290</v>
-      </c>
-      <c r="H69" t="s">
-        <v>82</v>
-      </c>
-      <c r="I69">
-        <v>2</v>
-      </c>
-      <c r="J69" s="7">
-        <v>4</v>
-      </c>
-      <c r="K69">
-        <v>2</v>
-      </c>
-      <c r="L69">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15">
+      <c r="L67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="E69" s="3"/>
+    </row>
+    <row r="70" spans="1:12">
       <c r="A70" t="s">
         <v>6</v>
       </c>
@@ -4697,31 +4734,31 @@
         <v>1.9</v>
       </c>
       <c r="D70">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E70">
-        <v>0.6</v>
+        <v>2.4</v>
       </c>
       <c r="F70">
-        <v>9152</v>
+        <v>9358</v>
       </c>
       <c r="H70" t="s">
         <v>82</v>
       </c>
       <c r="I70">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J70" s="7">
         <v>4</v>
       </c>
       <c r="K70">
+        <v>1</v>
+      </c>
+      <c r="L70">
         <v>4</v>
       </c>
-      <c r="L70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15">
+    </row>
+    <row r="71" spans="1:12">
       <c r="A71" t="s">
         <v>6</v>
       </c>
@@ -4732,177 +4769,173 @@
         <v>1.9</v>
       </c>
       <c r="D71">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E71">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
       <c r="F71">
-        <v>5804</v>
+        <v>5290</v>
       </c>
       <c r="H71" t="s">
         <v>82</v>
       </c>
       <c r="I71">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J71" s="7">
         <v>4</v>
       </c>
       <c r="K71">
+        <v>2</v>
+      </c>
+      <c r="L71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72">
+        <v>10</v>
+      </c>
+      <c r="C72" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="D72">
+        <v>16</v>
+      </c>
+      <c r="E72">
+        <v>0.6</v>
+      </c>
+      <c r="F72">
+        <v>9152</v>
+      </c>
+      <c r="H72" t="s">
+        <v>82</v>
+      </c>
+      <c r="I72">
+        <v>1</v>
+      </c>
+      <c r="J72" s="7">
         <v>4</v>
       </c>
-      <c r="L71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15">
-      <c r="C72" s="7"/>
-      <c r="J72" s="7"/>
-    </row>
-    <row r="73" spans="1:15">
-      <c r="C73" s="7"/>
-      <c r="J73" s="7"/>
-    </row>
-    <row r="74" spans="1:15">
+      <c r="K72">
+        <v>4</v>
+      </c>
+      <c r="L72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73">
+        <v>10</v>
+      </c>
+      <c r="C73" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="D73">
+        <v>16</v>
+      </c>
+      <c r="E73">
+        <v>0.6</v>
+      </c>
+      <c r="F73">
+        <v>5804</v>
+      </c>
+      <c r="H73" t="s">
+        <v>82</v>
+      </c>
+      <c r="I73">
+        <v>4</v>
+      </c>
+      <c r="J73" s="7">
+        <v>4</v>
+      </c>
+      <c r="K73">
+        <v>4</v>
+      </c>
+      <c r="L73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
       <c r="C74" s="7"/>
       <c r="J74" s="7"/>
     </row>
-    <row r="75" spans="1:15">
+    <row r="75" spans="1:12">
       <c r="C75" s="7"/>
       <c r="J75" s="7"/>
     </row>
-    <row r="76" spans="1:15">
+    <row r="76" spans="1:12">
       <c r="C76" s="7"/>
       <c r="J76" s="7"/>
     </row>
-    <row r="77" spans="1:15">
+    <row r="77" spans="1:12">
       <c r="C77" s="7"/>
       <c r="J77" s="7"/>
     </row>
-    <row r="78" spans="1:15" ht="20" thickBot="1">
-      <c r="A78" s="4" t="s">
+    <row r="78" spans="1:12">
+      <c r="C78" s="7"/>
+      <c r="J78" s="7"/>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="C79" s="7"/>
+      <c r="J79" s="7"/>
+    </row>
+    <row r="80" spans="1:12" ht="20" thickBot="1">
+      <c r="A80" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="50" thickTop="1" thickBot="1">
-      <c r="A79" s="1" t="s">
+    <row r="81" spans="1:15" ht="50" thickTop="1" thickBot="1">
+      <c r="A81" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C79" s="6" t="s">
+      <c r="B81" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E79" s="1" t="s">
+      <c r="E81" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F79" s="1" t="s">
+      <c r="F81" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G79" s="1" t="s">
+      <c r="G81" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H79" s="1" t="s">
+      <c r="H81" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I79" s="1" t="s">
+      <c r="I81" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J79" s="6" t="s">
+      <c r="J81" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K79" s="6" t="s">
+      <c r="K81" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L79" s="1" t="s">
+      <c r="L81" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M79" s="2" t="s">
+      <c r="M81" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="N79" s="2"/>
-      <c r="O79" s="2"/>
-    </row>
-    <row r="80" spans="1:15" ht="16" thickTop="1">
-      <c r="A80" t="s">
-        <v>6</v>
-      </c>
-      <c r="B80">
-        <v>40</v>
-      </c>
-      <c r="C80">
-        <v>1.9</v>
-      </c>
-      <c r="D80">
-        <v>40</v>
-      </c>
-      <c r="E80">
-        <v>0.20899999999999999</v>
-      </c>
-      <c r="G80">
-        <v>3966</v>
-      </c>
-      <c r="H80" t="s">
-        <v>47</v>
-      </c>
-      <c r="I80">
-        <v>2</v>
-      </c>
-      <c r="J80" s="7">
-        <v>80</v>
-      </c>
-      <c r="K80" s="8">
-        <v>10</v>
-      </c>
-      <c r="L80">
-        <v>2</v>
-      </c>
-      <c r="M80">
-        <v>105</v>
-      </c>
-      <c r="N80" s="3"/>
-    </row>
-    <row r="81" spans="1:14" ht="14" customHeight="1">
-      <c r="A81" t="s">
-        <v>6</v>
-      </c>
-      <c r="B81">
-        <v>40</v>
-      </c>
-      <c r="C81">
-        <v>1.9</v>
-      </c>
-      <c r="D81">
-        <v>20</v>
-      </c>
-      <c r="E81">
-        <v>0.435</v>
-      </c>
-      <c r="G81">
-        <v>8031</v>
-      </c>
-      <c r="H81" t="s">
-        <v>47</v>
-      </c>
-      <c r="I81">
-        <v>2</v>
-      </c>
-      <c r="J81" s="7">
-        <v>40</v>
-      </c>
-      <c r="K81" s="7">
-        <v>5</v>
-      </c>
-      <c r="L81">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14">
+      <c r="N81" s="2"/>
+      <c r="O81" s="2"/>
+    </row>
+    <row r="82" spans="1:15" ht="16" thickTop="1">
       <c r="A82" t="s">
         <v>6</v>
       </c>
@@ -4919,25 +4952,29 @@
         <v>0.20899999999999999</v>
       </c>
       <c r="G82">
-        <v>25807</v>
+        <v>3966</v>
       </c>
       <c r="H82" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="I82">
         <v>2</v>
       </c>
       <c r="J82" s="7">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="K82" s="8">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="L82">
         <v>2</v>
       </c>
-    </row>
-    <row r="83" spans="1:14">
+      <c r="M82">
+        <v>105</v>
+      </c>
+      <c r="N82" s="3"/>
+    </row>
+    <row r="83" spans="1:15" ht="14" customHeight="1">
       <c r="A83" t="s">
         <v>6</v>
       </c>
@@ -4954,25 +4991,25 @@
         <v>0.435</v>
       </c>
       <c r="G83">
-        <v>23872</v>
+        <v>8031</v>
       </c>
       <c r="H83" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="I83">
         <v>2</v>
       </c>
       <c r="J83" s="7">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="K83" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L83">
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:14">
+    <row r="84" spans="1:15">
       <c r="A84" t="s">
         <v>6</v>
       </c>
@@ -4988,23 +5025,26 @@
       <c r="E84">
         <v>0.20899999999999999</v>
       </c>
+      <c r="G84">
+        <v>25807</v>
+      </c>
       <c r="H84" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="I84">
         <v>2</v>
       </c>
       <c r="J84" s="7">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K84" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L84">
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:14">
+    <row r="85" spans="1:15">
       <c r="A85" t="s">
         <v>6</v>
       </c>
@@ -5020,28 +5060,31 @@
       <c r="E85">
         <v>0.435</v>
       </c>
+      <c r="G85">
+        <v>23872</v>
+      </c>
       <c r="H85" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="I85">
         <v>2</v>
       </c>
       <c r="J85" s="7">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K85" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L85">
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:14">
+    <row r="86" spans="1:15">
       <c r="A86" t="s">
         <v>6</v>
       </c>
       <c r="B86">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C86">
         <v>1.9</v>
@@ -5052,31 +5095,28 @@
       <c r="E86">
         <v>0.20899999999999999</v>
       </c>
-      <c r="G86">
-        <v>7337</v>
-      </c>
       <c r="H86" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="I86">
         <v>2</v>
       </c>
       <c r="J86" s="7">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="K86" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L86">
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:14">
+    <row r="87" spans="1:15">
       <c r="A87" t="s">
         <v>6</v>
       </c>
       <c r="B87">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C87">
         <v>1.9</v>
@@ -5088,159 +5128,151 @@
         <v>0.435</v>
       </c>
       <c r="H87" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="I87">
         <v>2</v>
       </c>
       <c r="J87" s="7">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="K87" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L87">
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:14">
-      <c r="J90" s="7"/>
-      <c r="K90" s="7"/>
-    </row>
-    <row r="91" spans="1:14">
-      <c r="K91" s="7"/>
-    </row>
-    <row r="92" spans="1:14" ht="20" thickBot="1">
-      <c r="A92" s="4" t="s">
+    <row r="88" spans="1:15">
+      <c r="A88" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88">
+        <v>10</v>
+      </c>
+      <c r="C88">
+        <v>1.9</v>
+      </c>
+      <c r="D88">
+        <v>40</v>
+      </c>
+      <c r="E88">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="G88">
+        <v>7337</v>
+      </c>
+      <c r="H88" t="s">
+        <v>5</v>
+      </c>
+      <c r="I88">
+        <v>2</v>
+      </c>
+      <c r="J88" s="7">
+        <v>12</v>
+      </c>
+      <c r="K88" s="8">
+        <v>3</v>
+      </c>
+      <c r="L88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15">
+      <c r="A89" t="s">
+        <v>6</v>
+      </c>
+      <c r="B89">
+        <v>10</v>
+      </c>
+      <c r="C89">
+        <v>1.9</v>
+      </c>
+      <c r="D89">
+        <v>20</v>
+      </c>
+      <c r="E89">
+        <v>0.435</v>
+      </c>
+      <c r="H89" t="s">
+        <v>5</v>
+      </c>
+      <c r="I89">
+        <v>2</v>
+      </c>
+      <c r="J89" s="7">
+        <v>12</v>
+      </c>
+      <c r="K89" s="7">
+        <v>3</v>
+      </c>
+      <c r="L89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15">
+      <c r="J92" s="7"/>
+      <c r="K92" s="7"/>
+    </row>
+    <row r="93" spans="1:15">
+      <c r="K93" s="7"/>
+    </row>
+    <row r="94" spans="1:15" ht="20" thickBot="1">
+      <c r="A94" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="K92" s="7"/>
-    </row>
-    <row r="93" spans="1:14" ht="50" thickTop="1" thickBot="1">
-      <c r="A93" s="1" t="s">
+      <c r="K94" s="7"/>
+    </row>
+    <row r="95" spans="1:15" ht="50" thickTop="1" thickBot="1">
+      <c r="A95" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C93" s="6" t="s">
+      <c r="B95" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="D95" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="E95" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F93" s="1" t="s">
+      <c r="F95" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G93" s="1" t="s">
+      <c r="G95" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H93" s="1" t="s">
+      <c r="H95" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I93" s="1" t="s">
+      <c r="I95" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J93" s="6" t="s">
+      <c r="J95" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K93" s="6" t="s">
+      <c r="K95" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L93" s="1" t="s">
+      <c r="L95" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M93" s="2" t="s">
+      <c r="M95" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="N93" s="2" t="s">
+      <c r="N95" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="16" thickTop="1">
-      <c r="A94" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B94" s="7">
-        <v>40</v>
-      </c>
-      <c r="C94">
-        <v>1.9</v>
-      </c>
-      <c r="D94" s="7">
-        <v>40</v>
-      </c>
-      <c r="E94" s="7">
-        <v>1</v>
-      </c>
-      <c r="F94" s="7">
-        <v>3468</v>
-      </c>
-      <c r="G94" s="7"/>
-      <c r="H94" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I94" s="7">
-        <v>2</v>
-      </c>
-      <c r="J94" s="7">
-        <v>2</v>
-      </c>
-      <c r="K94" s="8">
-        <v>0</v>
-      </c>
-      <c r="L94" s="7">
-        <v>2</v>
-      </c>
-      <c r="M94" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14">
-      <c r="A95" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B95" s="7">
-        <v>40</v>
-      </c>
-      <c r="C95">
-        <v>1.9</v>
-      </c>
-      <c r="D95" s="7">
-        <v>20</v>
-      </c>
-      <c r="E95" s="7">
-        <v>0.435</v>
-      </c>
-      <c r="G95" s="7"/>
-      <c r="H95" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I95" s="7">
-        <v>2</v>
-      </c>
-      <c r="J95" s="7">
-        <v>2</v>
-      </c>
-      <c r="K95" s="7">
-        <v>0</v>
-      </c>
-      <c r="L95" s="7">
-        <v>2</v>
-      </c>
-      <c r="M95" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14">
+    <row r="96" spans="1:15" ht="16" thickTop="1">
       <c r="A96" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B96" s="7">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C96">
         <v>1.9</v>
@@ -5249,16 +5281,14 @@
         <v>40</v>
       </c>
       <c r="E96" s="7">
-        <v>0.22900000000000001</v>
+        <v>1</v>
       </c>
       <c r="F96" s="7">
-        <v>907</v>
-      </c>
-      <c r="G96" s="7">
-        <v>1020</v>
-      </c>
+        <v>3468</v>
+      </c>
+      <c r="G96" s="7"/>
       <c r="H96" s="7" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="I96" s="7">
         <v>2</v>
@@ -5273,7 +5303,7 @@
         <v>2</v>
       </c>
       <c r="M96" s="7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="97" spans="1:13">
@@ -5281,22 +5311,20 @@
         <v>6</v>
       </c>
       <c r="B97" s="7">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C97">
         <v>1.9</v>
       </c>
       <c r="D97" s="7">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E97" s="7">
-        <v>0.22900000000000001</v>
-      </c>
-      <c r="G97" s="7">
-        <v>1080</v>
-      </c>
+        <v>0.435</v>
+      </c>
+      <c r="G97" s="7"/>
       <c r="H97" s="7" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="I97" s="7">
         <v>2</v>
@@ -5311,34 +5339,87 @@
         <v>2</v>
       </c>
       <c r="M97" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13">
+      <c r="A98" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B98" s="7">
+        <v>10</v>
+      </c>
+      <c r="C98">
+        <v>1.9</v>
+      </c>
+      <c r="D98" s="7">
+        <v>40</v>
+      </c>
+      <c r="E98" s="7">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="F98" s="7">
+        <v>907</v>
+      </c>
+      <c r="G98" s="7">
+        <v>1020</v>
+      </c>
+      <c r="H98" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I98" s="7">
+        <v>2</v>
+      </c>
+      <c r="J98" s="7">
+        <v>2</v>
+      </c>
+      <c r="K98" s="8">
+        <v>0</v>
+      </c>
+      <c r="L98" s="7">
+        <v>2</v>
+      </c>
+      <c r="M98" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13">
+      <c r="A99" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B99" s="7">
+        <v>10</v>
+      </c>
+      <c r="C99">
+        <v>1.9</v>
+      </c>
+      <c r="D99" s="7">
+        <v>40</v>
+      </c>
+      <c r="E99" s="7">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="G99" s="7">
+        <v>1080</v>
+      </c>
+      <c r="H99" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I99" s="7">
+        <v>2</v>
+      </c>
+      <c r="J99" s="7">
+        <v>2</v>
+      </c>
+      <c r="K99" s="7">
+        <v>0</v>
+      </c>
+      <c r="L99" s="7">
+        <v>2</v>
+      </c>
+      <c r="M99" s="7" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="98" spans="1:13">
-      <c r="A98" s="7"/>
-      <c r="B98" s="7"/>
-      <c r="D98" s="7"/>
-      <c r="E98" s="7"/>
-      <c r="G98" s="7"/>
-      <c r="H98" s="7"/>
-      <c r="I98" s="7"/>
-      <c r="J98" s="7"/>
-      <c r="K98" s="7"/>
-      <c r="L98" s="7"/>
-      <c r="M98" s="7"/>
-    </row>
-    <row r="99" spans="1:13">
-      <c r="A99" s="7"/>
-      <c r="B99" s="7"/>
-      <c r="D99" s="7"/>
-      <c r="E99" s="7"/>
-      <c r="G99" s="7"/>
-      <c r="H99" s="7"/>
-      <c r="I99" s="7"/>
-      <c r="J99" s="7"/>
-      <c r="K99" s="7"/>
-      <c r="L99" s="7"/>
-      <c r="M99" s="7"/>
     </row>
     <row r="100" spans="1:13">
       <c r="A100" s="7"/>
@@ -5353,258 +5434,218 @@
       <c r="L100" s="7"/>
       <c r="M100" s="7"/>
     </row>
-    <row r="103" spans="1:13" ht="20" thickBot="1">
-      <c r="A103" s="4" t="s">
+    <row r="101" spans="1:13">
+      <c r="A101" s="7"/>
+      <c r="B101" s="7"/>
+      <c r="D101" s="7"/>
+      <c r="E101" s="7"/>
+      <c r="G101" s="7"/>
+      <c r="H101" s="7"/>
+      <c r="I101" s="7"/>
+      <c r="J101" s="7"/>
+      <c r="K101" s="7"/>
+      <c r="L101" s="7"/>
+      <c r="M101" s="7"/>
+    </row>
+    <row r="102" spans="1:13">
+      <c r="A102" s="7"/>
+      <c r="B102" s="7"/>
+      <c r="D102" s="7"/>
+      <c r="E102" s="7"/>
+      <c r="G102" s="7"/>
+      <c r="H102" s="7"/>
+      <c r="I102" s="7"/>
+      <c r="J102" s="7"/>
+      <c r="K102" s="7"/>
+      <c r="L102" s="7"/>
+      <c r="M102" s="7"/>
+    </row>
+    <row r="105" spans="1:13" ht="20" thickBot="1">
+      <c r="A105" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="104" spans="1:13" ht="50" thickTop="1" thickBot="1">
-      <c r="A104" s="1" t="s">
+    <row r="106" spans="1:13" ht="50" thickTop="1" thickBot="1">
+      <c r="A106" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B104" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C104" s="6" t="s">
+      <c r="B106" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C106" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D106" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E104" s="1" t="s">
+      <c r="E106" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F104" s="1" t="s">
+      <c r="F106" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G104" s="1" t="s">
+      <c r="G106" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H104" s="1" t="s">
+      <c r="H106" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I104" s="1" t="s">
+      <c r="I106" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J104" s="6" t="s">
+      <c r="J106" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K104" s="6" t="s">
+      <c r="K106" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L104" s="1" t="s">
+      <c r="L106" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M104" s="2" t="s">
+      <c r="M106" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="1:13" ht="16" thickTop="1">
-      <c r="A105" s="7" t="s">
+    <row r="107" spans="1:13" ht="16" thickTop="1">
+      <c r="A107" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B105" s="7">
-        <v>40</v>
-      </c>
-      <c r="C105">
+      <c r="B107" s="7">
+        <v>40</v>
+      </c>
+      <c r="C107">
         <v>1.9</v>
       </c>
-      <c r="D105" s="7">
-        <v>40</v>
-      </c>
-      <c r="E105" s="7">
+      <c r="D107" s="7">
+        <v>40</v>
+      </c>
+      <c r="E107" s="7">
         <v>0.20899999999999999</v>
       </c>
-      <c r="G105" s="7"/>
-      <c r="H105" t="s">
+      <c r="G107" s="7"/>
+      <c r="H107" t="s">
         <v>42</v>
       </c>
-      <c r="I105" s="7">
+      <c r="I107" s="7">
         <v>2</v>
       </c>
-      <c r="J105" s="7">
+      <c r="J107" s="7">
         <v>80</v>
       </c>
-      <c r="K105" s="7">
+      <c r="K107" s="7">
         <v>10</v>
       </c>
-      <c r="M105" s="7" t="s">
+      <c r="M107" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="106" spans="1:13">
-      <c r="A106" s="7" t="s">
+    <row r="108" spans="1:13">
+      <c r="A108" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B106" s="7">
-        <v>40</v>
-      </c>
-      <c r="C106">
+      <c r="B108" s="7">
+        <v>40</v>
+      </c>
+      <c r="C108">
         <v>1.9</v>
       </c>
-      <c r="D106" s="7">
+      <c r="D108" s="7">
         <v>20</v>
       </c>
-      <c r="E106" s="7">
+      <c r="E108" s="7">
         <v>0.435</v>
       </c>
-      <c r="G106" s="7"/>
-      <c r="H106" t="s">
+      <c r="G108" s="7"/>
+      <c r="H108" t="s">
         <v>42</v>
       </c>
-      <c r="I106" s="7">
+      <c r="I108" s="7">
         <v>2</v>
       </c>
-      <c r="J106" s="7">
+      <c r="J108" s="7">
         <v>80</v>
       </c>
-      <c r="K106" s="7">
+      <c r="K108" s="7">
         <v>6</v>
       </c>
-      <c r="M106" s="7" t="s">
+      <c r="M108" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="111" spans="1:13" ht="20" thickBot="1">
-      <c r="A111" s="4" t="s">
+    <row r="113" spans="1:13" ht="20" thickBot="1">
+      <c r="A113" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="112" spans="1:13" ht="66" thickTop="1" thickBot="1">
-      <c r="A112" s="1" t="s">
+    <row r="114" spans="1:13" ht="66" thickTop="1" thickBot="1">
+      <c r="A114" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B112" s="11" t="s">
+      <c r="B114" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C114" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D112" s="6" t="s">
+      <c r="D114" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E112" s="1" t="s">
+      <c r="E114" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F112" s="1" t="s">
+      <c r="F114" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G112" s="11" t="s">
+      <c r="G114" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H112" s="11" t="s">
+      <c r="H114" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="I112" s="11"/>
-      <c r="J112" s="11" t="s">
+      <c r="I114" s="11"/>
+      <c r="J114" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="K112" s="11"/>
-      <c r="L112" s="12" t="s">
+      <c r="K114" s="11"/>
+      <c r="L114" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="16" thickTop="1">
-      <c r="A113" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B113">
-        <v>10</v>
-      </c>
-      <c r="C113" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D113">
-        <v>1.7</v>
-      </c>
-      <c r="E113" s="7">
-        <v>40</v>
-      </c>
-      <c r="F113" s="7">
-        <v>0.20899999999999999</v>
-      </c>
-      <c r="G113" s="7">
-        <v>0.105</v>
-      </c>
-      <c r="H113" s="7">
-        <v>54.6</v>
-      </c>
-      <c r="I113" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="J113" s="7">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="114" spans="1:13">
-      <c r="A114" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B114">
-        <v>10</v>
-      </c>
-      <c r="C114" t="s">
-        <v>63</v>
-      </c>
-      <c r="D114">
-        <v>1.7</v>
-      </c>
-      <c r="E114">
-        <v>40</v>
-      </c>
-      <c r="F114">
-        <v>0.20899999999999999</v>
-      </c>
-      <c r="G114">
-        <v>0.105</v>
-      </c>
-      <c r="H114" s="7">
-        <v>67</v>
-      </c>
-      <c r="I114" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="J114">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="115" spans="1:13">
+    <row r="115" spans="1:13" ht="16" thickTop="1">
       <c r="A115" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B115">
         <v>10</v>
       </c>
-      <c r="C115" t="s">
-        <v>63</v>
+      <c r="C115" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="D115">
         <v>1.7</v>
       </c>
-      <c r="E115">
-        <v>20</v>
-      </c>
-      <c r="F115">
-        <v>0.435</v>
-      </c>
-      <c r="G115">
-        <v>0.22</v>
-      </c>
-      <c r="H115">
-        <v>70</v>
+      <c r="E115" s="7">
+        <v>40</v>
+      </c>
+      <c r="F115" s="7">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="G115" s="7">
+        <v>0.105</v>
+      </c>
+      <c r="H115" s="7">
+        <v>54.6</v>
       </c>
       <c r="I115" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J115">
-        <v>1.6</v>
-      </c>
-      <c r="L115" s="12"/>
-      <c r="M115" s="3"/>
+      <c r="J115" s="7">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="116" spans="1:13">
-      <c r="A116" t="s">
-        <v>53</v>
+      <c r="A116" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="B116">
         <v>10</v>
@@ -5613,379 +5654,383 @@
         <v>63</v>
       </c>
       <c r="D116">
-        <v>0.435</v>
+        <v>1.7</v>
       </c>
       <c r="E116">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="F116">
-        <v>1</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="G116">
-        <v>0.2</v>
-      </c>
-      <c r="H116">
-        <v>20</v>
+        <v>0.105</v>
+      </c>
+      <c r="H116" s="7">
+        <v>67</v>
       </c>
       <c r="I116" s="3" t="s">
         <v>72</v>
       </c>
+      <c r="J116">
+        <v>1.6</v>
+      </c>
     </row>
     <row r="117" spans="1:13">
-      <c r="L117" s="3"/>
-    </row>
-    <row r="123" spans="1:13" ht="20" thickBot="1">
-      <c r="A123" s="4" t="s">
+      <c r="A117" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B117">
+        <v>10</v>
+      </c>
+      <c r="C117" t="s">
+        <v>63</v>
+      </c>
+      <c r="D117">
+        <v>1.7</v>
+      </c>
+      <c r="E117">
+        <v>20</v>
+      </c>
+      <c r="F117">
+        <v>0.435</v>
+      </c>
+      <c r="G117">
+        <v>0.22</v>
+      </c>
+      <c r="H117">
         <v>70</v>
       </c>
-    </row>
-    <row r="124" spans="1:13" ht="50" thickTop="1" thickBot="1">
-      <c r="A124" s="1" t="s">
+      <c r="I117" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J117">
+        <v>1.6</v>
+      </c>
+      <c r="L117" s="12"/>
+      <c r="M117" s="3"/>
+    </row>
+    <row r="118" spans="1:13">
+      <c r="A118" t="s">
+        <v>53</v>
+      </c>
+      <c r="B118">
+        <v>10</v>
+      </c>
+      <c r="C118" t="s">
+        <v>63</v>
+      </c>
+      <c r="D118">
+        <v>0.435</v>
+      </c>
+      <c r="E118">
+        <v>4</v>
+      </c>
+      <c r="F118">
+        <v>1</v>
+      </c>
+      <c r="G118">
+        <v>0.2</v>
+      </c>
+      <c r="H118">
+        <v>20</v>
+      </c>
+      <c r="I118" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13">
+      <c r="L119" s="3"/>
+    </row>
+    <row r="125" spans="1:13" ht="20" thickBot="1">
+      <c r="A125" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" ht="50" thickTop="1" thickBot="1">
+      <c r="A126" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B124" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C124" s="6" t="s">
+      <c r="B126" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C126" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D124" s="1" t="s">
+      <c r="D126" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E124" s="1" t="s">
+      <c r="E126" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F124" s="1" t="s">
+      <c r="F126" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G124" s="1" t="s">
+      <c r="G126" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H124" s="1" t="s">
+      <c r="H126" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I124" s="1" t="s">
+      <c r="I126" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J124" s="6" t="s">
+      <c r="J126" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K124" s="6" t="s">
+      <c r="K126" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="125" spans="1:13" ht="16" thickTop="1">
-      <c r="A125" t="s">
+    <row r="127" spans="1:13" ht="16" thickTop="1">
+      <c r="A127" t="s">
         <v>53</v>
       </c>
-      <c r="B125">
-        <v>40</v>
-      </c>
-      <c r="C125">
+      <c r="B127">
+        <v>40</v>
+      </c>
+      <c r="C127">
         <v>0.439</v>
       </c>
-      <c r="D125">
+      <c r="D127">
         <v>5</v>
       </c>
-      <c r="E125">
-        <v>1</v>
-      </c>
-      <c r="F125">
+      <c r="E127">
+        <v>1</v>
+      </c>
+      <c r="F127">
         <v>7464</v>
       </c>
-      <c r="H125" t="s">
+      <c r="H127" t="s">
         <v>55</v>
       </c>
-      <c r="I125">
-        <v>12</v>
-      </c>
-      <c r="J125" s="7">
-        <v>12</v>
-      </c>
-      <c r="K125" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="1:13">
-      <c r="A126" t="s">
+      <c r="I127">
+        <v>12</v>
+      </c>
+      <c r="J127" s="7">
+        <v>12</v>
+      </c>
+      <c r="K127" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13">
+      <c r="A128" t="s">
         <v>6</v>
       </c>
-      <c r="B126">
-        <v>40</v>
-      </c>
-      <c r="C126">
+      <c r="B128">
+        <v>40</v>
+      </c>
+      <c r="C128">
         <v>1.9</v>
       </c>
-      <c r="D126">
+      <c r="D128">
         <v>5</v>
       </c>
-      <c r="E126">
+      <c r="E128">
         <v>1.2</v>
       </c>
-      <c r="F126">
+      <c r="F128">
         <v>12960</v>
       </c>
-      <c r="H126" t="s">
+      <c r="H128" t="s">
         <v>55</v>
       </c>
-      <c r="I126">
-        <v>12</v>
-      </c>
-      <c r="J126" s="7">
-        <v>12</v>
-      </c>
-      <c r="K126" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="130" spans="1:11" ht="20" thickBot="1">
-      <c r="A130" s="4" t="s">
+      <c r="I128">
+        <v>12</v>
+      </c>
+      <c r="J128" s="7">
+        <v>12</v>
+      </c>
+      <c r="K128" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" ht="20" thickBot="1">
+      <c r="A132" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="131" spans="1:11" ht="50" thickTop="1" thickBot="1">
-      <c r="A131" s="1" t="s">
+    <row r="133" spans="1:11" ht="50" thickTop="1" thickBot="1">
+      <c r="A133" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B131" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C131" s="6" t="s">
+      <c r="B133" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C133" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D131" s="1" t="s">
+      <c r="D133" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E131" s="1" t="s">
+      <c r="E133" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F131" s="1" t="s">
+      <c r="F133" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G131" s="1" t="s">
+      <c r="G133" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H131" s="1" t="s">
+      <c r="H133" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I131" s="1" t="s">
+      <c r="I133" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J131" s="6" t="s">
+      <c r="J133" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K131" s="6" t="s">
+      <c r="K133" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="132" spans="1:11" ht="16" thickTop="1">
-      <c r="A132" t="s">
+    <row r="134" spans="1:11" ht="16" thickTop="1">
+      <c r="A134" t="s">
         <v>6</v>
       </c>
-      <c r="B132">
+      <c r="B134">
         <v>10</v>
       </c>
-      <c r="C132">
+      <c r="C134">
         <v>1.7</v>
       </c>
-      <c r="D132">
+      <c r="D134">
         <v>37</v>
       </c>
-      <c r="E132">
+      <c r="E134">
         <v>0.22900000000000001</v>
       </c>
-      <c r="F132">
+      <c r="F134">
         <v>662</v>
       </c>
-      <c r="H132" t="s">
+      <c r="H134" t="s">
         <v>7</v>
       </c>
-      <c r="I132">
-        <v>12</v>
-      </c>
-      <c r="J132" s="7">
-        <v>12</v>
-      </c>
-      <c r="K132" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133" spans="1:11">
-      <c r="A133" t="s">
+      <c r="I134">
+        <v>12</v>
+      </c>
+      <c r="J134" s="7">
+        <v>12</v>
+      </c>
+      <c r="K134" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11">
+      <c r="A135" t="s">
         <v>6</v>
       </c>
-      <c r="B133">
+      <c r="B135">
         <v>10</v>
       </c>
-      <c r="C133">
+      <c r="C135">
         <v>3.3</v>
       </c>
-      <c r="D133">
+      <c r="D135">
         <v>37</v>
       </c>
-      <c r="E133">
+      <c r="E135">
         <v>0.22900000000000001</v>
       </c>
-      <c r="F133">
+      <c r="F135">
         <v>676</v>
       </c>
-      <c r="H133" t="s">
+      <c r="H135" t="s">
         <v>7</v>
       </c>
-      <c r="I133">
-        <v>12</v>
-      </c>
-      <c r="J133" s="7">
-        <v>12</v>
-      </c>
-      <c r="K133" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" spans="1:11">
-      <c r="A139" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="142" spans="1:11">
-      <c r="A142" s="9" t="s">
+      <c r="I135">
+        <v>12</v>
+      </c>
+      <c r="J135" s="7">
+        <v>12</v>
+      </c>
+      <c r="K135" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11">
+      <c r="A141" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11">
+      <c r="A144" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="143" spans="1:11">
-      <c r="A143" s="9" t="s">
+    <row r="145" spans="1:12">
+      <c r="A145" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="144" spans="1:11" s="11" customFormat="1" ht="17" thickBot="1">
-      <c r="A144" s="9" t="s">
+    <row r="146" spans="1:12" s="11" customFormat="1" ht="17" thickBot="1">
+      <c r="A146" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B144"/>
-      <c r="C144"/>
-      <c r="D144"/>
-      <c r="E144"/>
-    </row>
-    <row r="145" spans="1:12" ht="16" thickTop="1">
-      <c r="A145" s="9" t="s">
+      <c r="B146"/>
+      <c r="C146"/>
+      <c r="D146"/>
+      <c r="E146"/>
+    </row>
+    <row r="147" spans="1:12" ht="16" thickTop="1">
+      <c r="A147" s="9" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="146" spans="1:12">
-      <c r="A146" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="147" spans="1:12">
-      <c r="A147" s="9" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="148" spans="1:12">
       <c r="A148" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12">
+      <c r="A149" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12">
+      <c r="A150" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="154" spans="1:12">
-      <c r="A154" s="9" t="s">
+    <row r="156" spans="1:12">
+      <c r="A156" s="9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="155" spans="1:12">
-      <c r="A155" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="156" spans="1:12" ht="18" customHeight="1">
-      <c r="A156" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L156" s="2"/>
     </row>
     <row r="157" spans="1:12">
       <c r="A157" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="158" spans="1:12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" ht="18" customHeight="1">
       <c r="A158" s="9" t="s">
-        <v>28</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="L158" s="2"/>
     </row>
     <row r="159" spans="1:12">
       <c r="A159" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="160" spans="1:12">
       <c r="A160" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12">
+      <c r="A161" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12">
+      <c r="A162" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="163" spans="1:12" ht="59" customHeight="1">
-      <c r="L163" s="2"/>
-    </row>
-    <row r="169" spans="1:12">
-      <c r="A169" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B169" s="7">
-        <v>10</v>
-      </c>
-      <c r="C169" s="7">
-        <v>0.435</v>
-      </c>
-      <c r="D169" s="7"/>
-      <c r="E169" s="7">
-        <v>0.19400000000000001</v>
-      </c>
-      <c r="F169" s="7">
-        <v>252</v>
-      </c>
-      <c r="G169" s="7"/>
-      <c r="H169" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="I169" s="7">
-        <v>12</v>
-      </c>
-      <c r="J169" s="7">
-        <v>12</v>
-      </c>
-      <c r="K169" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="170" spans="1:12">
-      <c r="A170" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B170" s="7">
-        <v>10</v>
-      </c>
-      <c r="C170" s="7">
-        <v>0.435</v>
-      </c>
-      <c r="D170" s="7"/>
-      <c r="E170" s="7">
-        <v>0.39</v>
-      </c>
-      <c r="F170" s="7">
-        <v>454</v>
-      </c>
-      <c r="G170" s="7"/>
-      <c r="H170" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="I170" s="7">
-        <v>12</v>
-      </c>
-      <c r="J170" s="7">
-        <v>12</v>
-      </c>
-      <c r="K170" s="7">
-        <v>1</v>
-      </c>
+    <row r="165" spans="1:12" ht="59" customHeight="1">
+      <c r="L165" s="2"/>
     </row>
     <row r="171" spans="1:12">
       <c r="A171" s="7" t="s">
@@ -5999,10 +6044,10 @@
       </c>
       <c r="D171" s="7"/>
       <c r="E171" s="7">
-        <v>0.58599999999999997</v>
+        <v>0.19400000000000001</v>
       </c>
       <c r="F171" s="7">
-        <v>700</v>
+        <v>252</v>
       </c>
       <c r="G171" s="7"/>
       <c r="H171" s="7" t="s">
@@ -6030,10 +6075,10 @@
       </c>
       <c r="D172" s="7"/>
       <c r="E172" s="7">
-        <v>0.78200000000000003</v>
+        <v>0.39</v>
       </c>
       <c r="F172" s="7">
-        <v>868</v>
+        <v>454</v>
       </c>
       <c r="G172" s="7"/>
       <c r="H172" s="7" t="s">
@@ -6061,10 +6106,10 @@
       </c>
       <c r="D173" s="7"/>
       <c r="E173" s="7">
-        <v>1</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="F173" s="7">
-        <v>1109</v>
+        <v>700</v>
       </c>
       <c r="G173" s="7"/>
       <c r="H173" s="7" t="s">
@@ -6092,9 +6137,11 @@
       </c>
       <c r="D174" s="7"/>
       <c r="E174" s="7">
-        <v>2</v>
-      </c>
-      <c r="F174" s="7"/>
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="F174" s="7">
+        <v>868</v>
+      </c>
       <c r="G174" s="7"/>
       <c r="H174" s="7" t="s">
         <v>55</v>
@@ -6110,36 +6157,90 @@
       </c>
     </row>
     <row r="175" spans="1:12">
-      <c r="A175" s="16" t="s">
+      <c r="A175" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B175" s="7">
+        <v>10</v>
+      </c>
+      <c r="C175" s="7">
+        <v>0.435</v>
+      </c>
+      <c r="D175" s="7"/>
+      <c r="E175" s="7">
+        <v>1</v>
+      </c>
+      <c r="F175" s="7">
+        <v>1109</v>
+      </c>
+      <c r="G175" s="7"/>
+      <c r="H175" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I175" s="7">
+        <v>12</v>
+      </c>
+      <c r="J175" s="7">
+        <v>12</v>
+      </c>
+      <c r="K175" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12">
+      <c r="A176" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B176" s="7">
+        <v>10</v>
+      </c>
+      <c r="C176" s="7">
+        <v>0.435</v>
+      </c>
+      <c r="D176" s="7"/>
+      <c r="E176" s="7">
+        <v>2</v>
+      </c>
+      <c r="F176" s="7"/>
+      <c r="G176" s="7"/>
+      <c r="H176" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I176" s="7">
+        <v>12</v>
+      </c>
+      <c r="J176" s="7">
+        <v>12</v>
+      </c>
+      <c r="K176" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11">
+      <c r="A177" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B175" s="16"/>
-      <c r="C175" s="7"/>
-      <c r="D175" s="7"/>
-      <c r="E175" s="7"/>
-      <c r="F175" s="7"/>
-      <c r="G175" s="7"/>
-      <c r="H175" s="7"/>
-      <c r="I175" s="7"/>
-      <c r="J175" s="7"/>
-      <c r="K175" s="7"/>
-    </row>
-    <row r="185" spans="1:1">
-      <c r="A185" s="10"/>
-    </row>
-    <row r="188" spans="1:1">
-      <c r="A188" s="9"/>
-    </row>
-    <row r="189" spans="1:1">
-      <c r="A189" s="9"/>
-    </row>
-    <row r="190" spans="1:1">
+      <c r="B177" s="16"/>
+      <c r="C177" s="7"/>
+      <c r="D177" s="7"/>
+      <c r="E177" s="7"/>
+      <c r="F177" s="7"/>
+      <c r="G177" s="7"/>
+      <c r="H177" s="7"/>
+      <c r="I177" s="7"/>
+      <c r="J177" s="7"/>
+      <c r="K177" s="7"/>
+    </row>
+    <row r="187" spans="1:11">
+      <c r="A187" s="10"/>
+    </row>
+    <row r="190" spans="1:11">
       <c r="A190" s="9"/>
     </row>
-    <row r="191" spans="1:1">
+    <row r="191" spans="1:11">
       <c r="A191" s="9"/>
     </row>
-    <row r="192" spans="1:1">
+    <row r="192" spans="1:11">
       <c r="A192" s="9"/>
     </row>
     <row r="193" spans="1:1">
@@ -6148,11 +6249,11 @@
     <row r="194" spans="1:1">
       <c r="A194" s="9"/>
     </row>
-    <row r="200" spans="1:1">
-      <c r="A200" s="9"/>
-    </row>
-    <row r="201" spans="1:1">
-      <c r="A201" s="9"/>
+    <row r="195" spans="1:1">
+      <c r="A195" s="9"/>
+    </row>
+    <row r="196" spans="1:1">
+      <c r="A196" s="9"/>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" s="9"/>
@@ -6169,8 +6270,15 @@
     <row r="206" spans="1:1">
       <c r="A206" s="9"/>
     </row>
+    <row r="207" spans="1:1">
+      <c r="A207" s="9"/>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
add a small table for slopes of three data sets (ttc vs. read size)
git-svn-id: file://localhost/tmp/svn2git/svn@4121 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/data-intensive-bio/Results.xlsx
+++ b/papers/data-intensive-bio/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="211" activeTab="1"/>
+    <workbookView xWindow="2960" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="211" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ranger" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8644" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8648" uniqueCount="107">
   <si>
     <t>Type</t>
   </si>
@@ -331,6 +331,18 @@
   <si>
     <t>HG 18 Chromosome 21</t>
   </si>
+  <si>
+    <t>Slopes</t>
+  </si>
+  <si>
+    <t>hg18-chr21</t>
+  </si>
+  <si>
+    <t>hg18</t>
+  </si>
+  <si>
+    <t>b.glumae</t>
+  </si>
 </sst>
 </file>
 
@@ -460,7 +472,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="404">
+  <cellStyleXfs count="406">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -865,6 +877,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -901,7 +915,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="404">
+  <cellStyles count="406">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1102,6 +1116,7 @@
     <cellStyle name="Followed Hyperlink" xfId="399" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="401" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="403" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="405" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="10" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
@@ -1304,6 +1319,7 @@
     <cellStyle name="Hyperlink" xfId="398" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="400" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="402" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="404" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Warning Text" xfId="79" builtinId="11"/>
   </cellStyles>
@@ -1489,11 +1505,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="651031400"/>
-        <c:axId val="650299176"/>
+        <c:axId val="408917144"/>
+        <c:axId val="404503352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="651031400"/>
+        <c:axId val="408917144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1526,12 +1542,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="650299176"/>
+        <c:crossAx val="404503352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="650299176"/>
+        <c:axId val="404503352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1575,7 +1591,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="651031400"/>
+        <c:crossAx val="408917144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1814,11 +1830,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="510472600"/>
-        <c:axId val="552016328"/>
+        <c:axId val="429978600"/>
+        <c:axId val="429984072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="510472600"/>
+        <c:axId val="429978600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1851,12 +1867,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="552016328"/>
+        <c:crossAx val="429984072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="552016328"/>
+        <c:axId val="429984072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1900,7 +1916,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="510472600"/>
+        <c:crossAx val="429978600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2108,11 +2124,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="534026264"/>
-        <c:axId val="698304568"/>
+        <c:axId val="430011608"/>
+        <c:axId val="430017208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="534026264"/>
+        <c:axId val="430011608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2145,12 +2161,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="698304568"/>
+        <c:crossAx val="430017208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="698304568"/>
+        <c:axId val="430017208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2194,7 +2210,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="534026264"/>
+        <c:crossAx val="430011608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2631,11 +2647,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="697837208"/>
-        <c:axId val="552025976"/>
+        <c:axId val="429943848"/>
+        <c:axId val="430079512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="697837208"/>
+        <c:axId val="429943848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2668,12 +2684,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="552025976"/>
+        <c:crossAx val="430079512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="552025976"/>
+        <c:axId val="430079512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2717,7 +2733,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="697837208"/>
+        <c:crossAx val="429943848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3133,11 +3149,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="654969992"/>
-        <c:axId val="534731128"/>
+        <c:axId val="408818936"/>
+        <c:axId val="408824648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="654969992"/>
+        <c:axId val="408818936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3165,12 +3181,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="534731128"/>
+        <c:crossAx val="408824648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="534731128"/>
+        <c:axId val="408824648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3203,7 +3219,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="654969992"/>
+        <c:crossAx val="408818936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3550,11 +3566,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="534415752"/>
-        <c:axId val="551772472"/>
+        <c:axId val="404984920"/>
+        <c:axId val="404990488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="534415752"/>
+        <c:axId val="404984920"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -3583,12 +3599,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="551772472"/>
+        <c:crossAx val="404990488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="551772472"/>
+        <c:axId val="404990488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3616,7 +3632,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="534415752"/>
+        <c:crossAx val="404984920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3770,11 +3786,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="534614344"/>
-        <c:axId val="510596712"/>
+        <c:axId val="404998136"/>
+        <c:axId val="429940456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="534614344"/>
+        <c:axId val="404998136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3784,13 +3800,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="510596712"/>
+        <c:crossAx val="429940456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="510596712"/>
+        <c:axId val="429940456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3800,7 +3816,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="534614344"/>
+        <c:crossAx val="404998136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4745,10 +4761,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="O129" sqref="O129"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="V29" sqref="V29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5136,7 +5152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:25">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -5165,7 +5181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:25">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -5195,7 +5211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:25">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -5224,7 +5240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:25">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -5253,7 +5269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:25">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -5282,7 +5298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:25">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -5311,7 +5327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:25">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -5339,8 +5355,11 @@
       <c r="I24" s="7">
         <v>1</v>
       </c>
+      <c r="W24" t="s">
+        <v>103</v>
+      </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:25">
       <c r="A25" s="7" t="s">
         <v>79</v>
       </c>
@@ -5369,7 +5388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:25">
       <c r="A26" s="7" t="s">
         <v>79</v>
       </c>
@@ -5397,11 +5416,37 @@
       <c r="I26" s="7">
         <v>1</v>
       </c>
+      <c r="V26" t="s">
+        <v>104</v>
+      </c>
+      <c r="W26">
+        <v>2672.6</v>
+      </c>
+      <c r="X26">
+        <v>11371</v>
+      </c>
+      <c r="Y26">
+        <f>+X26/W26</f>
+        <v>4.2546583850931681</v>
+      </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:25">
       <c r="A27" s="15"/>
+      <c r="V27" t="s">
+        <v>105</v>
+      </c>
+      <c r="W27">
+        <v>5129</v>
+      </c>
+      <c r="X27">
+        <v>17912</v>
+      </c>
+      <c r="Y27">
+        <f t="shared" ref="Y27:Y28" si="0">+X27/W27</f>
+        <v>3.4922986937024763</v>
+      </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:25">
       <c r="A28" t="s">
         <v>101</v>
       </c>
@@ -5429,8 +5474,21 @@
       <c r="I28" s="7">
         <v>1</v>
       </c>
+      <c r="V28" t="s">
+        <v>106</v>
+      </c>
+      <c r="W28">
+        <v>1674.5</v>
+      </c>
+      <c r="X28">
+        <v>7462.8</v>
+      </c>
+      <c r="Y28">
+        <f t="shared" si="0"/>
+        <v>4.4567333532397733</v>
+      </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:25">
       <c r="A29" t="s">
         <v>101</v>
       </c>
@@ -5459,7 +5517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:25">
       <c r="A30" t="s">
         <v>101</v>
       </c>
@@ -5488,7 +5546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:25">
       <c r="A31" t="s">
         <v>101</v>
       </c>
@@ -5517,7 +5575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:25">
       <c r="A32" s="15"/>
     </row>
     <row r="33" spans="1:9">
@@ -5644,6 +5702,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
adding more description for the table showing slopes and ratios
git-svn-id: file://localhost/tmp/svn2git/svn@4127 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/data-intensive-bio/Results.xlsx
+++ b/papers/data-intensive-bio/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="211" activeTab="1"/>
+    <workbookView xWindow="1380" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="211" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ranger" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8648" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8651" uniqueCount="110">
   <si>
     <t>Type</t>
   </si>
@@ -332,9 +332,6 @@
     <t>HG 18 Chromosome 21</t>
   </si>
   <si>
-    <t>Slopes</t>
-  </si>
-  <si>
     <t>hg18-chr21</t>
   </si>
   <si>
@@ -342,6 +339,18 @@
   </si>
   <si>
     <t>b.glumae</t>
+  </si>
+  <si>
+    <t>10 index</t>
+  </si>
+  <si>
+    <t>40 index</t>
+  </si>
+  <si>
+    <t>slope ratio</t>
+  </si>
+  <si>
+    <t>SLOPES</t>
   </si>
 </sst>
 </file>
@@ -1505,11 +1514,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="408917144"/>
-        <c:axId val="404503352"/>
+        <c:axId val="381279880"/>
+        <c:axId val="381140104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="408917144"/>
+        <c:axId val="381279880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1542,12 +1551,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="404503352"/>
+        <c:crossAx val="381140104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="404503352"/>
+        <c:axId val="381140104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1591,7 +1600,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408917144"/>
+        <c:crossAx val="381279880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1830,11 +1839,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="429978600"/>
-        <c:axId val="429984072"/>
+        <c:axId val="405413912"/>
+        <c:axId val="390991912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="429978600"/>
+        <c:axId val="405413912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1867,12 +1876,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="429984072"/>
+        <c:crossAx val="390991912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="429984072"/>
+        <c:axId val="390991912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1916,7 +1925,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="429978600"/>
+        <c:crossAx val="405413912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2124,11 +2133,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="430011608"/>
-        <c:axId val="430017208"/>
+        <c:axId val="386350056"/>
+        <c:axId val="386355656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="430011608"/>
+        <c:axId val="386350056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2161,12 +2170,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="430017208"/>
+        <c:crossAx val="386355656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="430017208"/>
+        <c:axId val="386355656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2210,7 +2219,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="430011608"/>
+        <c:crossAx val="386350056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2276,7 +2285,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2403,7 +2411,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2647,11 +2654,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="429943848"/>
-        <c:axId val="430079512"/>
+        <c:axId val="430034328"/>
+        <c:axId val="430039976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="429943848"/>
+        <c:axId val="430034328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2677,19 +2684,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="430079512"/>
+        <c:crossAx val="430039976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="430079512"/>
+        <c:axId val="430039976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2726,14 +2732,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="429943848"/>
+        <c:crossAx val="430034328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3149,11 +3154,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="408818936"/>
-        <c:axId val="408824648"/>
+        <c:axId val="429989736"/>
+        <c:axId val="429995448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="408818936"/>
+        <c:axId val="429989736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3181,12 +3186,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408824648"/>
+        <c:crossAx val="429995448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="408824648"/>
+        <c:axId val="429995448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3219,7 +3224,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="408818936"/>
+        <c:crossAx val="429989736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3566,11 +3571,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="404984920"/>
-        <c:axId val="404990488"/>
+        <c:axId val="408891256"/>
+        <c:axId val="390095384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="404984920"/>
+        <c:axId val="408891256"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -3599,12 +3604,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="404990488"/>
+        <c:crossAx val="390095384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="404990488"/>
+        <c:axId val="390095384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3632,7 +3637,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="404984920"/>
+        <c:crossAx val="408891256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3786,11 +3791,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="404998136"/>
-        <c:axId val="429940456"/>
+        <c:axId val="405158600"/>
+        <c:axId val="404972040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="404998136"/>
+        <c:axId val="405158600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3800,13 +3805,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="429940456"/>
+        <c:crossAx val="404972040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="429940456"/>
+        <c:axId val="404972040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3816,7 +3821,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="404998136"/>
+        <c:crossAx val="405158600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4763,8 +4768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="V29" sqref="V29"/>
+    <sheetView tabSelected="1" topLeftCell="H2" workbookViewId="0">
+      <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5356,7 +5361,7 @@
         <v>1</v>
       </c>
       <c r="W24" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:25">
@@ -5387,6 +5392,15 @@
       <c r="I25" s="7">
         <v>1</v>
       </c>
+      <c r="W25" t="s">
+        <v>106</v>
+      </c>
+      <c r="X25" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="26" spans="1:25">
       <c r="A26" s="7" t="s">
@@ -5417,7 +5431,7 @@
         <v>1</v>
       </c>
       <c r="V26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="W26">
         <v>2672.6</v>
@@ -5433,7 +5447,7 @@
     <row r="27" spans="1:25">
       <c r="A27" s="15"/>
       <c r="V27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="W27">
         <v>5129</v>
@@ -5475,7 +5489,7 @@
         <v>1</v>
       </c>
       <c r="V28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="W28">
         <v>1674.5</v>
@@ -5702,7 +5716,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>